<commit_message>
Updated RMI files - Nathan's edits
</commit_message>
<xml_diff>
--- a/InputData/bldgs/DSCF/Distributed Solar Cap Factor.xlsx
+++ b/InputData/bldgs/DSCF/Distributed Solar Cap Factor.xlsx
@@ -1664,7 +1664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39"/>
   </cellStyleXfs>
-  <cellXfs count="307">
+  <cellXfs count="304">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -2115,7 +2115,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2130,9 +2129,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="113" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -2213,9 +2209,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="111" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="124" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -2224,6 +2217,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -5900,18 +5961,6 @@
           <t>Current Costs</t>
         </is>
       </c>
-      <c r="H10" s="252" t="n"/>
-      <c r="I10" s="252" t="n"/>
-      <c r="J10" s="252" t="n"/>
-      <c r="K10" s="252" t="n"/>
-      <c r="L10" s="252" t="n"/>
-      <c r="M10" s="252" t="n"/>
-      <c r="N10" s="252" t="n"/>
-      <c r="O10" s="252" t="n"/>
-      <c r="P10" s="252" t="n"/>
-      <c r="Q10" s="252" t="n"/>
-      <c r="R10" s="252" t="n"/>
-      <c r="S10" s="252" t="n"/>
       <c r="T10" s="29" t="n"/>
       <c r="U10" s="16" t="n"/>
       <c r="V10" s="16" t="n"/>
@@ -6034,13 +6083,13 @@
       <c r="E12" s="16" t="n"/>
       <c r="F12" s="16" t="n"/>
       <c r="G12" s="30" t="n"/>
-      <c r="H12" s="253" t="inlineStr">
+      <c r="H12" s="252" t="inlineStr">
         <is>
           <t>Techno-Economic Cost and Performance Parameters</t>
         </is>
       </c>
       <c r="I12" s="16" t="n"/>
-      <c r="J12" s="254" t="inlineStr">
+      <c r="J12" s="253" t="inlineStr">
         <is>
           <t>Net Capacity Factor (%)</t>
         </is>
@@ -6055,18 +6104,18 @@
       </c>
       <c r="M12" s="16" t="n"/>
       <c r="N12" s="16" t="n"/>
-      <c r="O12" s="255" t="inlineStr">
+      <c r="O12" s="254" t="inlineStr">
         <is>
           <t>Basis Year:</t>
         </is>
       </c>
-      <c r="P12" s="256" t="n"/>
-      <c r="Q12" s="257" t="n">
+      <c r="P12" s="255" t="n"/>
+      <c r="Q12" s="256" t="n">
         <v>2017</v>
       </c>
-      <c r="R12" s="258" t="n"/>
-      <c r="S12" s="258" t="n"/>
-      <c r="T12" s="256" t="n"/>
+      <c r="R12" s="257" t="n"/>
+      <c r="S12" s="257" t="n"/>
+      <c r="T12" s="255" t="n"/>
       <c r="U12" s="16" t="n"/>
       <c r="V12" s="16" t="n"/>
       <c r="W12" s="16" t="n"/>
@@ -6121,9 +6170,7 @@
       <c r="E13" s="16" t="n"/>
       <c r="F13" s="16" t="n"/>
       <c r="G13" s="30" t="n"/>
-      <c r="H13" s="252" t="n"/>
       <c r="I13" s="16" t="n"/>
-      <c r="J13" s="252" t="n"/>
       <c r="K13" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -6194,9 +6241,7 @@
       <c r="E14" s="16" t="n"/>
       <c r="F14" s="16" t="n"/>
       <c r="G14" s="30" t="n"/>
-      <c r="H14" s="252" t="n"/>
       <c r="I14" s="16" t="n"/>
-      <c r="J14" s="252" t="n"/>
       <c r="K14" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -6207,22 +6252,18 @@
       </c>
       <c r="M14" s="16" t="n"/>
       <c r="N14" s="16" t="n"/>
-      <c r="O14" s="259" t="inlineStr">
+      <c r="O14" s="258" t="inlineStr">
         <is>
           <t>Residential Solar Photovoltaic</t>
         </is>
       </c>
-      <c r="P14" s="258" t="n"/>
-      <c r="Q14" s="258" t="n"/>
-      <c r="R14" s="258" t="n"/>
-      <c r="S14" s="258" t="n"/>
-      <c r="T14" s="256" t="n"/>
+      <c r="P14" s="257" t="n"/>
+      <c r="Q14" s="257" t="n"/>
+      <c r="R14" s="257" t="n"/>
+      <c r="S14" s="257" t="n"/>
+      <c r="T14" s="255" t="n"/>
       <c r="U14" s="16" t="n"/>
-      <c r="V14" s="260" t="n"/>
-      <c r="W14" s="252" t="n"/>
-      <c r="X14" s="252" t="n"/>
-      <c r="Y14" s="252" t="n"/>
-      <c r="Z14" s="252" t="n"/>
+      <c r="V14" s="44" t="n"/>
       <c r="AA14" s="16" t="n"/>
       <c r="AB14" s="16" t="n"/>
       <c r="AC14" s="16" t="n"/>
@@ -6271,9 +6312,7 @@
       <c r="E15" s="16" t="n"/>
       <c r="F15" s="16" t="n"/>
       <c r="G15" s="30" t="n"/>
-      <c r="H15" s="252" t="n"/>
       <c r="I15" s="16" t="n"/>
-      <c r="J15" s="252" t="n"/>
       <c r="K15" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -6291,8 +6330,6 @@
       <c r="S15" s="46" t="n"/>
       <c r="T15" s="47" t="n"/>
       <c r="U15" s="16" t="n"/>
-      <c r="V15" s="252" t="n"/>
-      <c r="Z15" s="252" t="n"/>
       <c r="AA15" s="16" t="n"/>
       <c r="AB15" s="16" t="n"/>
       <c r="AC15" s="16" t="n"/>
@@ -6341,9 +6378,7 @@
       <c r="E16" s="16" t="n"/>
       <c r="F16" s="16" t="n"/>
       <c r="G16" s="30" t="n"/>
-      <c r="H16" s="252" t="n"/>
       <c r="I16" s="16" t="n"/>
-      <c r="J16" s="252" t="n"/>
       <c r="K16" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -6361,8 +6396,6 @@
       <c r="S16" s="46" t="n"/>
       <c r="T16" s="47" t="n"/>
       <c r="U16" s="16" t="n"/>
-      <c r="V16" s="252" t="n"/>
-      <c r="Z16" s="252" t="n"/>
       <c r="AA16" s="16" t="n"/>
       <c r="AB16" s="16" t="n"/>
       <c r="AC16" s="16" t="n"/>
@@ -6411,26 +6444,23 @@
       <c r="E17" s="16" t="n"/>
       <c r="F17" s="16" t="n"/>
       <c r="G17" s="30" t="n"/>
-      <c r="H17" s="252" t="n"/>
       <c r="I17" s="16" t="n"/>
       <c r="J17" s="49" t="n"/>
       <c r="K17" s="16" t="n"/>
       <c r="L17" s="16" t="n"/>
       <c r="M17" s="16" t="n"/>
       <c r="N17" s="16" t="n"/>
-      <c r="O17" s="261" t="inlineStr">
+      <c r="O17" s="259" t="inlineStr">
         <is>
           <t>Representative Dist. Res system is fixed-tilt roof mounted  with capacity of 5 kW</t>
         </is>
       </c>
-      <c r="P17" s="262" t="n"/>
-      <c r="Q17" s="262" t="n"/>
-      <c r="R17" s="262" t="n"/>
-      <c r="S17" s="262" t="n"/>
-      <c r="T17" s="263" t="n"/>
+      <c r="P17" s="260" t="n"/>
+      <c r="Q17" s="260" t="n"/>
+      <c r="R17" s="260" t="n"/>
+      <c r="S17" s="260" t="n"/>
+      <c r="T17" s="261" t="n"/>
       <c r="U17" s="16" t="n"/>
-      <c r="V17" s="252" t="n"/>
-      <c r="Z17" s="252" t="n"/>
       <c r="AA17" s="16" t="n"/>
       <c r="AB17" s="16" t="n"/>
       <c r="AC17" s="16" t="n"/>
@@ -6479,9 +6509,8 @@
       <c r="E18" s="16" t="n"/>
       <c r="F18" s="16" t="n"/>
       <c r="G18" s="30" t="n"/>
-      <c r="H18" s="252" t="n"/>
       <c r="I18" s="16" t="n"/>
-      <c r="J18" s="254" t="inlineStr">
+      <c r="J18" s="253" t="inlineStr">
         <is>
           <t>Annual Energy Production (kWh/kW)</t>
         </is>
@@ -6497,19 +6526,13 @@
       </c>
       <c r="M18" s="16" t="n"/>
       <c r="N18" s="16" t="n"/>
-      <c r="O18" s="264" t="inlineStr">
+      <c r="O18" s="262" t="inlineStr">
         <is>
           <t xml:space="preserve">Overnight Capital Cost, Capacity Factor, Fixed O&amp;M, and Variable O&amp;M costs </t>
         </is>
       </c>
-      <c r="P18" s="252" t="n"/>
-      <c r="Q18" s="252" t="n"/>
-      <c r="R18" s="252" t="n"/>
-      <c r="S18" s="252" t="n"/>
-      <c r="T18" s="265" t="n"/>
+      <c r="T18" s="263" t="n"/>
       <c r="U18" s="16" t="n"/>
-      <c r="V18" s="252" t="n"/>
-      <c r="Z18" s="252" t="n"/>
       <c r="AA18" s="16" t="n"/>
       <c r="AB18" s="16" t="n"/>
       <c r="AC18" s="16" t="n"/>
@@ -6558,9 +6581,7 @@
       <c r="E19" s="16" t="n"/>
       <c r="F19" s="16" t="n"/>
       <c r="G19" s="30" t="n"/>
-      <c r="H19" s="252" t="n"/>
       <c r="I19" s="16" t="n"/>
-      <c r="J19" s="252" t="n"/>
       <c r="K19" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -6572,19 +6593,13 @@
       </c>
       <c r="M19" s="16" t="n"/>
       <c r="N19" s="16" t="n"/>
-      <c r="O19" s="264" t="inlineStr">
+      <c r="O19" s="262" t="inlineStr">
         <is>
           <t>represent $/kW DC;  however LCOE reflects $/MWh AC.</t>
         </is>
       </c>
-      <c r="P19" s="252" t="n"/>
-      <c r="Q19" s="252" t="n"/>
-      <c r="R19" s="252" t="n"/>
-      <c r="S19" s="252" t="n"/>
-      <c r="T19" s="265" t="n"/>
+      <c r="T19" s="263" t="n"/>
       <c r="U19" s="16" t="n"/>
-      <c r="V19" s="252" t="n"/>
-      <c r="Z19" s="252" t="n"/>
       <c r="AA19" s="16" t="n"/>
       <c r="AB19" s="16" t="n"/>
       <c r="AC19" s="16" t="n"/>
@@ -6633,9 +6648,7 @@
       <c r="E20" s="16" t="n"/>
       <c r="F20" s="16" t="n"/>
       <c r="G20" s="30" t="n"/>
-      <c r="H20" s="252" t="n"/>
       <c r="I20" s="16" t="n"/>
-      <c r="J20" s="252" t="n"/>
       <c r="K20" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -6647,19 +6660,17 @@
       </c>
       <c r="M20" s="16" t="n"/>
       <c r="N20" s="16" t="n"/>
-      <c r="O20" s="266" t="inlineStr">
+      <c r="O20" s="264" t="inlineStr">
         <is>
           <t>Capacity factors chosen here to reflect range of across the continental U.S. using NREL PVWATTS</t>
         </is>
       </c>
-      <c r="P20" s="262" t="n"/>
-      <c r="Q20" s="262" t="n"/>
-      <c r="R20" s="262" t="n"/>
-      <c r="S20" s="262" t="n"/>
-      <c r="T20" s="263" t="n"/>
+      <c r="P20" s="260" t="n"/>
+      <c r="Q20" s="260" t="n"/>
+      <c r="R20" s="260" t="n"/>
+      <c r="S20" s="260" t="n"/>
+      <c r="T20" s="261" t="n"/>
       <c r="U20" s="16" t="n"/>
-      <c r="V20" s="252" t="n"/>
-      <c r="Z20" s="252" t="n"/>
       <c r="AA20" s="16" t="n"/>
       <c r="AB20" s="16" t="n"/>
       <c r="AC20" s="16" t="n"/>
@@ -6708,9 +6719,7 @@
       <c r="E21" s="16" t="n"/>
       <c r="F21" s="16" t="n"/>
       <c r="G21" s="30" t="n"/>
-      <c r="H21" s="252" t="n"/>
       <c r="I21" s="16" t="n"/>
-      <c r="J21" s="252" t="n"/>
       <c r="K21" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -6729,8 +6738,6 @@
       <c r="S21" s="58" t="n"/>
       <c r="T21" s="59" t="n"/>
       <c r="U21" s="16" t="n"/>
-      <c r="V21" s="252" t="n"/>
-      <c r="Z21" s="252" t="n"/>
       <c r="AA21" s="16" t="n"/>
       <c r="AB21" s="16" t="n"/>
       <c r="AC21" s="16" t="n"/>
@@ -6779,9 +6786,7 @@
       <c r="E22" s="16" t="n"/>
       <c r="F22" s="16" t="n"/>
       <c r="G22" s="30" t="n"/>
-      <c r="H22" s="252" t="n"/>
       <c r="I22" s="16" t="n"/>
-      <c r="J22" s="252" t="n"/>
       <c r="K22" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -6800,8 +6805,6 @@
       <c r="S22" s="58" t="n"/>
       <c r="T22" s="59" t="n"/>
       <c r="U22" s="16" t="n"/>
-      <c r="V22" s="252" t="n"/>
-      <c r="Z22" s="252" t="n"/>
       <c r="AA22" s="16" t="n"/>
       <c r="AB22" s="16" t="n"/>
       <c r="AC22" s="16" t="n"/>
@@ -6850,17 +6853,16 @@
       <c r="E23" s="16" t="n"/>
       <c r="F23" s="16" t="n"/>
       <c r="G23" s="30" t="n"/>
-      <c r="H23" s="252" t="n"/>
       <c r="I23" s="16" t="n"/>
       <c r="J23" s="49" t="n"/>
       <c r="K23" s="16" t="n"/>
       <c r="L23" s="16" t="n"/>
       <c r="M23" s="16" t="n"/>
       <c r="N23" s="16" t="n"/>
-      <c r="O23" s="267" t="n"/>
-      <c r="P23" s="268" t="n"/>
-      <c r="Q23" s="268" t="n"/>
-      <c r="R23" s="269" t="n"/>
+      <c r="O23" s="265" t="n"/>
+      <c r="P23" s="266" t="n"/>
+      <c r="Q23" s="266" t="n"/>
+      <c r="R23" s="267" t="n"/>
       <c r="S23" s="63" t="inlineStr">
         <is>
           <t>Available</t>
@@ -6872,8 +6874,6 @@
         </is>
       </c>
       <c r="U23" s="16" t="n"/>
-      <c r="V23" s="252" t="n"/>
-      <c r="Z23" s="252" t="n"/>
       <c r="AA23" s="16" t="n"/>
       <c r="AB23" s="16" t="n"/>
       <c r="AC23" s="16" t="n"/>
@@ -6922,9 +6922,8 @@
       <c r="E24" s="16" t="n"/>
       <c r="F24" s="16" t="n"/>
       <c r="G24" s="30" t="n"/>
-      <c r="H24" s="252" t="n"/>
       <c r="I24" s="16" t="n"/>
-      <c r="J24" s="254" t="inlineStr">
+      <c r="J24" s="253" t="inlineStr">
         <is>
           <t>CAPEX ($/kW)</t>
         </is>
@@ -6940,8 +6939,8 @@
       </c>
       <c r="M24" s="16" t="n"/>
       <c r="N24" s="16" t="n"/>
-      <c r="O24" s="270" t="n"/>
-      <c r="R24" s="265" t="n"/>
+      <c r="O24" s="268" t="n"/>
+      <c r="R24" s="263" t="n"/>
       <c r="S24" s="66" t="inlineStr">
         <is>
           <t>Capacity</t>
@@ -6953,8 +6952,6 @@
         </is>
       </c>
       <c r="U24" s="16" t="n"/>
-      <c r="V24" s="252" t="n"/>
-      <c r="Z24" s="252" t="n"/>
       <c r="AA24" s="16" t="n"/>
       <c r="AB24" s="16" t="n"/>
       <c r="AC24" s="16" t="n"/>
@@ -7003,9 +7000,7 @@
       <c r="E25" s="16" t="n"/>
       <c r="F25" s="16" t="n"/>
       <c r="G25" s="30" t="n"/>
-      <c r="H25" s="252" t="n"/>
       <c r="I25" s="16" t="n"/>
-      <c r="J25" s="252" t="n"/>
       <c r="K25" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -7017,10 +7012,8 @@
       </c>
       <c r="M25" s="16" t="n"/>
       <c r="N25" s="16" t="n"/>
-      <c r="O25" s="270" t="n"/>
-      <c r="P25" s="252" t="n"/>
-      <c r="Q25" s="252" t="n"/>
-      <c r="R25" s="265" t="n"/>
+      <c r="O25" s="268" t="n"/>
+      <c r="R25" s="263" t="n"/>
       <c r="S25" s="66" t="inlineStr">
         <is>
           <t>(GW)</t>
@@ -7032,8 +7025,6 @@
         </is>
       </c>
       <c r="U25" s="16" t="n"/>
-      <c r="V25" s="252" t="n"/>
-      <c r="Z25" s="252" t="n"/>
       <c r="AA25" s="16" t="n"/>
       <c r="AB25" s="16" t="n"/>
       <c r="AC25" s="16" t="n"/>
@@ -7082,9 +7073,7 @@
       <c r="E26" s="16" t="n"/>
       <c r="F26" s="16" t="n"/>
       <c r="G26" s="30" t="n"/>
-      <c r="H26" s="252" t="n"/>
       <c r="I26" s="16" t="n"/>
-      <c r="J26" s="252" t="n"/>
       <c r="K26" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -7097,9 +7086,9 @@
       <c r="M26" s="16" t="n"/>
       <c r="N26" s="16" t="n"/>
       <c r="O26" s="68" t="n"/>
-      <c r="P26" s="262" t="n"/>
-      <c r="Q26" s="262" t="n"/>
-      <c r="R26" s="262" t="n"/>
+      <c r="P26" s="260" t="n"/>
+      <c r="Q26" s="260" t="n"/>
+      <c r="R26" s="260" t="n"/>
       <c r="S26" s="69" t="n">
         <v>731</v>
       </c>
@@ -7107,8 +7096,6 @@
         <v>926000</v>
       </c>
       <c r="U26" s="16" t="n"/>
-      <c r="V26" s="252" t="n"/>
-      <c r="Z26" s="252" t="n"/>
       <c r="AA26" s="16" t="n"/>
       <c r="AB26" s="16" t="n"/>
       <c r="AC26" s="16" t="n"/>
@@ -7157,9 +7144,7 @@
       <c r="E27" s="16" t="n"/>
       <c r="F27" s="16" t="n"/>
       <c r="G27" s="30" t="n"/>
-      <c r="H27" s="252" t="n"/>
       <c r="I27" s="16" t="n"/>
-      <c r="J27" s="252" t="n"/>
       <c r="K27" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -7178,8 +7163,6 @@
       <c r="S27" s="72" t="n"/>
       <c r="T27" s="73" t="n"/>
       <c r="U27" s="16" t="n"/>
-      <c r="V27" s="252" t="n"/>
-      <c r="Z27" s="252" t="n"/>
       <c r="AA27" s="16" t="n"/>
       <c r="AB27" s="16" t="n"/>
       <c r="AC27" s="16" t="n"/>
@@ -7228,9 +7211,7 @@
       <c r="E28" s="16" t="n"/>
       <c r="F28" s="16" t="n"/>
       <c r="G28" s="30" t="n"/>
-      <c r="H28" s="252" t="n"/>
       <c r="I28" s="16" t="n"/>
-      <c r="J28" s="252" t="n"/>
       <c r="K28" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -7249,8 +7230,6 @@
       <c r="S28" s="72" t="n"/>
       <c r="T28" s="73" t="n"/>
       <c r="U28" s="16" t="n"/>
-      <c r="V28" s="252" t="n"/>
-      <c r="Z28" s="252" t="n"/>
       <c r="AA28" s="16" t="n"/>
       <c r="AB28" s="16" t="n"/>
       <c r="AC28" s="16" t="n"/>
@@ -7299,7 +7278,6 @@
       <c r="E29" s="16" t="n"/>
       <c r="F29" s="16" t="n"/>
       <c r="G29" s="30" t="n"/>
-      <c r="H29" s="252" t="n"/>
       <c r="I29" s="16" t="n"/>
       <c r="J29" s="16" t="n"/>
       <c r="K29" s="16" t="n"/>
@@ -7311,18 +7289,16 @@
           <t>Res PV - Seattle</t>
         </is>
       </c>
-      <c r="P29" s="268" t="n"/>
-      <c r="Q29" s="271" t="inlineStr">
+      <c r="P29" s="266" t="n"/>
+      <c r="Q29" s="269" t="inlineStr">
         <is>
           <t>ATB values reflect annual average capacity factor over life of plant including estimated degradation, starting at  0.75% per year, reducing to 0.3% and 0.5% annual degradation by 2050 for the low- and mid-cases.</t>
         </is>
       </c>
-      <c r="R29" s="268" t="n"/>
-      <c r="S29" s="268" t="n"/>
-      <c r="T29" s="269" t="n"/>
+      <c r="R29" s="266" t="n"/>
+      <c r="S29" s="266" t="n"/>
+      <c r="T29" s="267" t="n"/>
       <c r="U29" s="16" t="n"/>
-      <c r="V29" s="252" t="n"/>
-      <c r="Z29" s="252" t="n"/>
       <c r="AA29" s="16" t="n"/>
       <c r="AB29" s="16" t="n"/>
       <c r="AC29" s="16" t="n"/>
@@ -7371,9 +7347,8 @@
       <c r="E30" s="16" t="n"/>
       <c r="F30" s="16" t="n"/>
       <c r="G30" s="30" t="n"/>
-      <c r="H30" s="252" t="n"/>
       <c r="I30" s="16" t="n"/>
-      <c r="J30" s="254" t="inlineStr">
+      <c r="J30" s="253" t="inlineStr">
         <is>
           <t>Construction Financing Cost ($/kW)</t>
         </is>
@@ -7394,12 +7369,9 @@
           <t>Res PV - Chicago</t>
         </is>
       </c>
-      <c r="P30" s="252" t="n"/>
-      <c r="Q30" s="270" t="n"/>
-      <c r="T30" s="265" t="n"/>
+      <c r="Q30" s="268" t="n"/>
+      <c r="T30" s="263" t="n"/>
       <c r="U30" s="16" t="n"/>
-      <c r="V30" s="252" t="n"/>
-      <c r="Z30" s="252" t="n"/>
       <c r="AA30" s="16" t="n"/>
       <c r="AB30" s="16" t="n"/>
       <c r="AC30" s="16" t="n"/>
@@ -7448,9 +7420,7 @@
       <c r="E31" s="16" t="n"/>
       <c r="F31" s="16" t="n"/>
       <c r="G31" s="30" t="n"/>
-      <c r="H31" s="252" t="n"/>
       <c r="I31" s="16" t="n"/>
-      <c r="J31" s="252" t="n"/>
       <c r="K31" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -7467,12 +7437,9 @@
           <t>Res PV - Kansas City</t>
         </is>
       </c>
-      <c r="P31" s="252" t="n"/>
-      <c r="Q31" s="270" t="n"/>
-      <c r="T31" s="265" t="n"/>
+      <c r="Q31" s="268" t="n"/>
+      <c r="T31" s="263" t="n"/>
       <c r="U31" s="16" t="n"/>
-      <c r="V31" s="252" t="n"/>
-      <c r="Z31" s="252" t="n"/>
       <c r="AA31" s="16" t="n"/>
       <c r="AB31" s="16" t="n"/>
       <c r="AC31" s="16" t="n"/>
@@ -7521,9 +7488,7 @@
       <c r="E32" s="16" t="n"/>
       <c r="F32" s="16" t="n"/>
       <c r="G32" s="30" t="n"/>
-      <c r="H32" s="252" t="n"/>
       <c r="I32" s="16" t="n"/>
-      <c r="J32" s="252" t="n"/>
       <c r="K32" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -7545,11 +7510,9 @@
           <t>Res PV - Los Angeles</t>
         </is>
       </c>
-      <c r="Q32" s="270" t="n"/>
-      <c r="T32" s="265" t="n"/>
+      <c r="Q32" s="268" t="n"/>
+      <c r="T32" s="263" t="n"/>
       <c r="U32" s="16" t="n"/>
-      <c r="V32" s="252" t="n"/>
-      <c r="Z32" s="252" t="n"/>
       <c r="AA32" s="16" t="n"/>
       <c r="AB32" s="16" t="n"/>
       <c r="AC32" s="16" t="n"/>
@@ -7598,9 +7561,7 @@
       <c r="E33" s="16" t="n"/>
       <c r="F33" s="16" t="n"/>
       <c r="G33" s="30" t="n"/>
-      <c r="H33" s="252" t="n"/>
       <c r="I33" s="16" t="n"/>
-      <c r="J33" s="252" t="n"/>
       <c r="K33" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -7622,13 +7583,11 @@
           <t>Res PV - Daggett, CA</t>
         </is>
       </c>
-      <c r="Q33" s="272" t="n"/>
-      <c r="R33" s="262" t="n"/>
-      <c r="S33" s="262" t="n"/>
-      <c r="T33" s="263" t="n"/>
+      <c r="Q33" s="270" t="n"/>
+      <c r="R33" s="260" t="n"/>
+      <c r="S33" s="260" t="n"/>
+      <c r="T33" s="261" t="n"/>
       <c r="U33" s="16" t="n"/>
-      <c r="V33" s="252" t="n"/>
-      <c r="Z33" s="252" t="n"/>
       <c r="AA33" s="16" t="n"/>
       <c r="AB33" s="16" t="n"/>
       <c r="AC33" s="16" t="n"/>
@@ -7677,9 +7636,7 @@
       <c r="E34" s="16" t="n"/>
       <c r="F34" s="16" t="n"/>
       <c r="G34" s="30" t="n"/>
-      <c r="H34" s="252" t="n"/>
       <c r="I34" s="16" t="n"/>
-      <c r="J34" s="252" t="n"/>
       <c r="K34" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -7698,8 +7655,6 @@
       <c r="S34" s="16" t="n"/>
       <c r="T34" s="31" t="n"/>
       <c r="U34" s="16" t="n"/>
-      <c r="V34" s="252" t="n"/>
-      <c r="Z34" s="252" t="n"/>
       <c r="AA34" s="16" t="n"/>
       <c r="AB34" s="16" t="n"/>
       <c r="AC34" s="16" t="n"/>
@@ -7748,29 +7703,23 @@
       <c r="E35" s="16" t="n"/>
       <c r="F35" s="16" t="n"/>
       <c r="G35" s="30" t="n"/>
-      <c r="H35" s="252" t="n"/>
       <c r="I35" s="16" t="n"/>
       <c r="J35" s="16" t="n"/>
       <c r="K35" s="16" t="n"/>
       <c r="L35" s="16" t="n"/>
       <c r="M35" s="16" t="n"/>
       <c r="N35" s="16" t="n"/>
-      <c r="O35" s="273" t="inlineStr">
+      <c r="O35" s="271" t="inlineStr">
         <is>
           <t>Financial Assumptions:</t>
         </is>
       </c>
-      <c r="P35" s="274" t="n"/>
-      <c r="Q35" s="274" t="n"/>
-      <c r="R35" s="274" t="n"/>
-      <c r="S35" s="275" t="n"/>
+      <c r="P35" s="272" t="n"/>
+      <c r="Q35" s="272" t="n"/>
+      <c r="R35" s="272" t="n"/>
+      <c r="S35" s="273" t="n"/>
       <c r="T35" s="31" t="n"/>
       <c r="U35" s="16" t="n"/>
-      <c r="V35" s="252" t="n"/>
-      <c r="W35" s="252" t="n"/>
-      <c r="X35" s="252" t="n"/>
-      <c r="Y35" s="252" t="n"/>
-      <c r="Z35" s="252" t="n"/>
       <c r="AA35" s="16" t="n"/>
       <c r="AB35" s="16" t="n"/>
       <c r="AC35" s="16" t="n"/>
@@ -7819,9 +7768,8 @@
       <c r="E36" s="16" t="n"/>
       <c r="F36" s="16" t="n"/>
       <c r="G36" s="30" t="n"/>
-      <c r="H36" s="252" t="n"/>
       <c r="I36" s="16" t="n"/>
-      <c r="J36" s="254" t="inlineStr">
+      <c r="J36" s="253" t="inlineStr">
         <is>
           <t>Overnight Capital Cost ($/kW)</t>
         </is>
@@ -7842,9 +7790,9 @@
           <t>Inflation Rate</t>
         </is>
       </c>
-      <c r="P36" s="276" t="n"/>
-      <c r="Q36" s="276" t="n"/>
-      <c r="R36" s="276" t="n"/>
+      <c r="P36" s="274" t="n"/>
+      <c r="Q36" s="274" t="n"/>
+      <c r="R36" s="274" t="n"/>
       <c r="S36" s="87">
         <f>L203</f>
         <v/>
@@ -7904,9 +7852,7 @@
       <c r="E37" s="16" t="n"/>
       <c r="F37" s="16" t="n"/>
       <c r="G37" s="30" t="n"/>
-      <c r="H37" s="252" t="n"/>
       <c r="I37" s="16" t="n"/>
-      <c r="J37" s="252" t="n"/>
       <c r="K37" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -7923,9 +7869,9 @@
           <t>Capital Recovery Period (Years)</t>
         </is>
       </c>
-      <c r="P37" s="277" t="n"/>
-      <c r="Q37" s="277" t="n"/>
-      <c r="R37" s="277" t="n"/>
+      <c r="P37" s="275" t="n"/>
+      <c r="Q37" s="275" t="n"/>
+      <c r="R37" s="275" t="n"/>
       <c r="S37" s="90" t="n">
         <v>30</v>
       </c>
@@ -7984,9 +7930,7 @@
       <c r="E38" s="16" t="n"/>
       <c r="F38" s="16" t="n"/>
       <c r="G38" s="30" t="n"/>
-      <c r="H38" s="252" t="n"/>
       <c r="I38" s="16" t="n"/>
-      <c r="J38" s="252" t="n"/>
       <c r="K38" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -8003,9 +7947,9 @@
           <t>Interest Rate Nominal - Mid</t>
         </is>
       </c>
-      <c r="P38" s="277" t="n"/>
-      <c r="Q38" s="277" t="n"/>
-      <c r="R38" s="277" t="n"/>
+      <c r="P38" s="275" t="n"/>
+      <c r="Q38" s="275" t="n"/>
+      <c r="R38" s="275" t="n"/>
       <c r="S38" s="91">
         <f>L205</f>
         <v/>
@@ -8065,9 +8009,7 @@
       <c r="E39" s="16" t="n"/>
       <c r="F39" s="16" t="n"/>
       <c r="G39" s="30" t="n"/>
-      <c r="H39" s="252" t="n"/>
       <c r="I39" s="16" t="n"/>
-      <c r="J39" s="252" t="n"/>
       <c r="K39" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -8139,9 +8081,7 @@
       <c r="E40" s="16" t="n"/>
       <c r="F40" s="16" t="n"/>
       <c r="G40" s="30" t="n"/>
-      <c r="H40" s="252" t="n"/>
       <c r="I40" s="16" t="n"/>
-      <c r="J40" s="252" t="n"/>
       <c r="K40" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -8213,7 +8153,6 @@
       <c r="E41" s="16" t="n"/>
       <c r="F41" s="16" t="n"/>
       <c r="G41" s="30" t="n"/>
-      <c r="H41" s="252" t="n"/>
       <c r="I41" s="16" t="n"/>
       <c r="J41" s="16" t="n"/>
       <c r="K41" s="16" t="n"/>
@@ -8225,9 +8164,9 @@
           <t>Calculated Interest Rate Real - Mid</t>
         </is>
       </c>
-      <c r="P41" s="277" t="n"/>
-      <c r="Q41" s="277" t="n"/>
-      <c r="R41" s="277" t="n"/>
+      <c r="P41" s="275" t="n"/>
+      <c r="Q41" s="275" t="n"/>
+      <c r="R41" s="275" t="n"/>
       <c r="S41" s="93">
         <f>L208</f>
         <v/>
@@ -8287,9 +8226,8 @@
       <c r="E42" s="16" t="n"/>
       <c r="F42" s="16" t="n"/>
       <c r="G42" s="30" t="n"/>
-      <c r="H42" s="252" t="n"/>
       <c r="I42" s="16" t="n"/>
-      <c r="J42" s="254" t="inlineStr">
+      <c r="J42" s="253" t="inlineStr">
         <is>
           <t>Fixed Operation and Maintenance Expenses ($/kW/yr)</t>
         </is>
@@ -8310,9 +8248,9 @@
           <t>Interest During Construction  - Nominal</t>
         </is>
       </c>
-      <c r="P42" s="277" t="n"/>
-      <c r="Q42" s="277" t="n"/>
-      <c r="R42" s="277" t="n"/>
+      <c r="P42" s="275" t="n"/>
+      <c r="Q42" s="275" t="n"/>
+      <c r="R42" s="275" t="n"/>
       <c r="S42" s="91">
         <f>L210</f>
         <v/>
@@ -8372,9 +8310,7 @@
       <c r="E43" s="16" t="n"/>
       <c r="F43" s="16" t="n"/>
       <c r="G43" s="30" t="n"/>
-      <c r="H43" s="252" t="n"/>
       <c r="I43" s="16" t="n"/>
-      <c r="J43" s="252" t="n"/>
       <c r="K43" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -8391,9 +8327,9 @@
           <t>Rate of Return on Equity Nominal - Mid</t>
         </is>
       </c>
-      <c r="P43" s="277" t="n"/>
-      <c r="Q43" s="277" t="n"/>
-      <c r="R43" s="277" t="n"/>
+      <c r="P43" s="275" t="n"/>
+      <c r="Q43" s="275" t="n"/>
+      <c r="R43" s="275" t="n"/>
       <c r="S43" s="91">
         <f>L212</f>
         <v/>
@@ -8457,9 +8393,7 @@
       <c r="E44" s="16" t="n"/>
       <c r="F44" s="16" t="n"/>
       <c r="G44" s="30" t="n"/>
-      <c r="H44" s="252" t="n"/>
       <c r="I44" s="16" t="n"/>
-      <c r="J44" s="252" t="n"/>
       <c r="K44" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -8476,9 +8410,9 @@
           <t>Calculated Rate of Return on Equity Real - Mid</t>
         </is>
       </c>
-      <c r="P44" s="277" t="n"/>
-      <c r="Q44" s="277" t="n"/>
-      <c r="R44" s="277" t="n"/>
+      <c r="P44" s="275" t="n"/>
+      <c r="Q44" s="275" t="n"/>
+      <c r="R44" s="275" t="n"/>
       <c r="S44" s="93">
         <f>L215</f>
         <v/>
@@ -8538,9 +8472,7 @@
       <c r="E45" s="16" t="n"/>
       <c r="F45" s="16" t="n"/>
       <c r="G45" s="30" t="n"/>
-      <c r="H45" s="252" t="n"/>
       <c r="I45" s="16" t="n"/>
-      <c r="J45" s="252" t="n"/>
       <c r="K45" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -8612,9 +8544,7 @@
       <c r="E46" s="16" t="n"/>
       <c r="F46" s="16" t="n"/>
       <c r="G46" s="30" t="n"/>
-      <c r="H46" s="252" t="n"/>
       <c r="I46" s="16" t="n"/>
-      <c r="J46" s="252" t="n"/>
       <c r="K46" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -8686,7 +8616,6 @@
       <c r="E47" s="16" t="n"/>
       <c r="F47" s="16" t="n"/>
       <c r="G47" s="30" t="n"/>
-      <c r="H47" s="252" t="n"/>
       <c r="I47" s="16" t="n"/>
       <c r="J47" s="16" t="n"/>
       <c r="K47" s="42" t="n"/>
@@ -8698,9 +8627,9 @@
           <t>Debt Fraction - Mid</t>
         </is>
       </c>
-      <c r="P47" s="277" t="n"/>
-      <c r="Q47" s="277" t="n"/>
-      <c r="R47" s="277" t="n"/>
+      <c r="P47" s="275" t="n"/>
+      <c r="Q47" s="275" t="n"/>
+      <c r="R47" s="275" t="n"/>
       <c r="S47" s="91">
         <f>L218</f>
         <v/>
@@ -8760,9 +8689,8 @@
       <c r="E48" s="16" t="n"/>
       <c r="F48" s="16" t="n"/>
       <c r="G48" s="30" t="n"/>
-      <c r="H48" s="252" t="n"/>
       <c r="I48" s="16" t="n"/>
-      <c r="J48" s="254" t="inlineStr">
+      <c r="J48" s="253" t="inlineStr">
         <is>
           <t>Variable Operation and Maintenance Expenses ($/MWh)</t>
         </is>
@@ -8782,9 +8710,9 @@
           <t>Tax Rate (Federal and State)</t>
         </is>
       </c>
-      <c r="P48" s="277" t="n"/>
-      <c r="Q48" s="277" t="n"/>
-      <c r="R48" s="277" t="n"/>
+      <c r="P48" s="275" t="n"/>
+      <c r="Q48" s="275" t="n"/>
+      <c r="R48" s="275" t="n"/>
       <c r="S48" s="91">
         <f>L220</f>
         <v/>
@@ -8844,9 +8772,7 @@
       <c r="E49" s="16" t="n"/>
       <c r="F49" s="16" t="n"/>
       <c r="G49" s="30" t="n"/>
-      <c r="H49" s="252" t="n"/>
       <c r="I49" s="16" t="n"/>
-      <c r="J49" s="252" t="n"/>
       <c r="K49" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -8862,9 +8788,9 @@
           <t>WACC Nominal - Mid</t>
         </is>
       </c>
-      <c r="P49" s="277" t="n"/>
-      <c r="Q49" s="277" t="n"/>
-      <c r="R49" s="277" t="n"/>
+      <c r="P49" s="275" t="n"/>
+      <c r="Q49" s="275" t="n"/>
+      <c r="R49" s="275" t="n"/>
       <c r="S49" s="93">
         <f>L222</f>
         <v/>
@@ -8924,9 +8850,7 @@
       <c r="E50" s="16" t="n"/>
       <c r="F50" s="16" t="n"/>
       <c r="G50" s="30" t="n"/>
-      <c r="H50" s="252" t="n"/>
       <c r="I50" s="16" t="n"/>
-      <c r="J50" s="252" t="n"/>
       <c r="K50" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -8942,9 +8866,9 @@
           <t>WACC Real - Mid</t>
         </is>
       </c>
-      <c r="P50" s="277" t="n"/>
-      <c r="Q50" s="277" t="n"/>
-      <c r="R50" s="277" t="n"/>
+      <c r="P50" s="275" t="n"/>
+      <c r="Q50" s="275" t="n"/>
+      <c r="R50" s="275" t="n"/>
       <c r="S50" s="93">
         <f>L225</f>
         <v/>
@@ -9004,9 +8928,7 @@
       <c r="E51" s="16" t="n"/>
       <c r="F51" s="16" t="n"/>
       <c r="G51" s="30" t="n"/>
-      <c r="H51" s="252" t="n"/>
       <c r="I51" s="16" t="n"/>
-      <c r="J51" s="252" t="n"/>
       <c r="K51" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -9077,9 +8999,7 @@
       <c r="E52" s="16" t="n"/>
       <c r="F52" s="16" t="n"/>
       <c r="G52" s="30" t="n"/>
-      <c r="H52" s="252" t="n"/>
       <c r="I52" s="16" t="n"/>
-      <c r="J52" s="252" t="n"/>
       <c r="K52" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -9162,9 +9082,9 @@
           <t>Depreciation Period</t>
         </is>
       </c>
-      <c r="P53" s="277" t="n"/>
-      <c r="Q53" s="277" t="n"/>
-      <c r="R53" s="277" t="n"/>
+      <c r="P53" s="275" t="n"/>
+      <c r="Q53" s="275" t="n"/>
+      <c r="R53" s="275" t="n"/>
       <c r="S53" s="99" t="n">
         <v>5</v>
       </c>
@@ -9235,9 +9155,9 @@
           <t>Construction Finance Factor</t>
         </is>
       </c>
-      <c r="P54" s="277" t="n"/>
-      <c r="Q54" s="277" t="n"/>
-      <c r="R54" s="277" t="n"/>
+      <c r="P54" s="275" t="n"/>
+      <c r="Q54" s="275" t="n"/>
+      <c r="R54" s="275" t="n"/>
       <c r="S54" s="103" t="n">
         <v>1</v>
       </c>
@@ -9296,13 +9216,13 @@
       <c r="E55" s="16" t="n"/>
       <c r="F55" s="16" t="n"/>
       <c r="G55" s="30" t="n"/>
-      <c r="H55" s="278" t="inlineStr">
+      <c r="H55" s="276" t="inlineStr">
         <is>
           <t>Finance</t>
         </is>
       </c>
       <c r="I55" s="16" t="n"/>
-      <c r="J55" s="254" t="inlineStr">
+      <c r="J55" s="253" t="inlineStr">
         <is>
           <t>Weighted Average Cost of Capital (WACC) (Nominal) (%)</t>
         </is>
@@ -9323,9 +9243,9 @@
           <t>Present Value of Depreciation</t>
         </is>
       </c>
-      <c r="P55" s="277" t="n"/>
-      <c r="Q55" s="277" t="n"/>
-      <c r="R55" s="277" t="n"/>
+      <c r="P55" s="275" t="n"/>
+      <c r="Q55" s="275" t="n"/>
+      <c r="R55" s="275" t="n"/>
       <c r="S55" s="103">
         <f>SUMPRODUCT(O74:T74,O76:T76)</f>
         <v/>
@@ -9385,9 +9305,7 @@
       <c r="E56" s="16" t="n"/>
       <c r="F56" s="16" t="n"/>
       <c r="G56" s="30" t="n"/>
-      <c r="H56" s="252" t="n"/>
       <c r="I56" s="16" t="n"/>
-      <c r="J56" s="252" t="n"/>
       <c r="K56" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -9404,9 +9322,9 @@
           <t>Project Finance Factor</t>
         </is>
       </c>
-      <c r="P56" s="277" t="n"/>
-      <c r="Q56" s="277" t="n"/>
-      <c r="R56" s="277" t="n"/>
+      <c r="P56" s="275" t="n"/>
+      <c r="Q56" s="275" t="n"/>
+      <c r="R56" s="275" t="n"/>
       <c r="S56" s="103">
         <f> (1 - S48 * S55) / (1 - S48)</f>
         <v/>
@@ -9466,9 +9384,7 @@
       <c r="E57" s="16" t="n"/>
       <c r="F57" s="16" t="n"/>
       <c r="G57" s="30" t="n"/>
-      <c r="H57" s="252" t="n"/>
       <c r="I57" s="16" t="n"/>
-      <c r="J57" s="252" t="n"/>
       <c r="K57" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -9485,9 +9401,9 @@
           <t>Capital Recovery Factor (CRF) Nominal - Mid</t>
         </is>
       </c>
-      <c r="P57" s="277" t="n"/>
-      <c r="Q57" s="277" t="n"/>
-      <c r="R57" s="277" t="n"/>
+      <c r="P57" s="275" t="n"/>
+      <c r="Q57" s="275" t="n"/>
+      <c r="R57" s="275" t="n"/>
       <c r="S57" s="93">
         <f>L228</f>
         <v/>
@@ -9547,9 +9463,7 @@
       <c r="E58" s="16" t="n"/>
       <c r="F58" s="16" t="n"/>
       <c r="G58" s="30" t="n"/>
-      <c r="H58" s="252" t="n"/>
       <c r="I58" s="16" t="n"/>
-      <c r="J58" s="252" t="n"/>
       <c r="K58" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -9621,9 +9535,7 @@
       <c r="E59" s="16" t="n"/>
       <c r="F59" s="16" t="n"/>
       <c r="G59" s="30" t="n"/>
-      <c r="H59" s="252" t="n"/>
       <c r="I59" s="16" t="n"/>
-      <c r="J59" s="252" t="n"/>
       <c r="K59" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -9707,9 +9619,9 @@
           <t>Capital Recovery Factor (CRF) Real - Mid</t>
         </is>
       </c>
-      <c r="P60" s="279" t="n"/>
-      <c r="Q60" s="279" t="n"/>
-      <c r="R60" s="279" t="n"/>
+      <c r="P60" s="277" t="n"/>
+      <c r="Q60" s="277" t="n"/>
+      <c r="R60" s="277" t="n"/>
       <c r="S60" s="112">
         <f>L231</f>
         <v/>
@@ -9836,13 +9748,13 @@
       <c r="E62" s="16" t="n"/>
       <c r="F62" s="16" t="n"/>
       <c r="G62" s="30" t="n"/>
-      <c r="H62" s="280" t="inlineStr">
+      <c r="H62" s="278" t="inlineStr">
         <is>
           <t>Grid Connection Costs</t>
         </is>
       </c>
       <c r="I62" s="16" t="n"/>
-      <c r="J62" s="254" t="inlineStr">
+      <c r="J62" s="253" t="inlineStr">
         <is>
           <t>Grid Connection Costs (GCC) ($/kW)</t>
         </is>
@@ -9863,7 +9775,7 @@
           <t>Construction Duration yrs</t>
         </is>
       </c>
-      <c r="P62" s="274" t="n"/>
+      <c r="P62" s="272" t="n"/>
       <c r="Q62" s="117" t="n">
         <v>0</v>
       </c>
@@ -9924,9 +9836,7 @@
       <c r="E63" s="16" t="n"/>
       <c r="F63" s="16" t="n"/>
       <c r="G63" s="30" t="n"/>
-      <c r="H63" s="252" t="n"/>
       <c r="I63" s="16" t="n"/>
-      <c r="J63" s="252" t="n"/>
       <c r="K63" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -10010,9 +9920,7 @@
       <c r="E64" s="16" t="n"/>
       <c r="F64" s="16" t="n"/>
       <c r="G64" s="30" t="n"/>
-      <c r="H64" s="252" t="n"/>
       <c r="I64" s="16" t="n"/>
-      <c r="J64" s="252" t="n"/>
       <c r="K64" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -10096,9 +10004,7 @@
       <c r="E65" s="16" t="n"/>
       <c r="F65" s="16" t="n"/>
       <c r="G65" s="30" t="n"/>
-      <c r="H65" s="252" t="n"/>
       <c r="I65" s="16" t="n"/>
-      <c r="J65" s="252" t="n"/>
       <c r="K65" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -10170,9 +10076,7 @@
       <c r="E66" s="16" t="n"/>
       <c r="F66" s="16" t="n"/>
       <c r="G66" s="30" t="n"/>
-      <c r="H66" s="252" t="n"/>
       <c r="I66" s="16" t="n"/>
-      <c r="J66" s="252" t="n"/>
       <c r="K66" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -10244,7 +10148,6 @@
       <c r="E67" s="16" t="n"/>
       <c r="F67" s="16" t="n"/>
       <c r="G67" s="30" t="n"/>
-      <c r="H67" s="252" t="n"/>
       <c r="I67" s="16" t="n"/>
       <c r="J67" s="16" t="n"/>
       <c r="K67" s="16" t="n"/>
@@ -10318,9 +10221,8 @@
       <c r="E68" s="16" t="n"/>
       <c r="F68" s="16" t="n"/>
       <c r="G68" s="30" t="n"/>
-      <c r="H68" s="252" t="n"/>
       <c r="I68" s="16" t="n"/>
-      <c r="J68" s="254" t="inlineStr">
+      <c r="J68" s="253" t="inlineStr">
         <is>
           <t>Grid Feature Costs ($/kW)</t>
         </is>
@@ -10402,9 +10304,7 @@
       <c r="E69" s="16" t="n"/>
       <c r="F69" s="16" t="n"/>
       <c r="G69" s="30" t="n"/>
-      <c r="H69" s="252" t="n"/>
       <c r="I69" s="16" t="n"/>
-      <c r="J69" s="252" t="n"/>
       <c r="K69" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -10482,9 +10382,7 @@
       <c r="E70" s="16" t="n"/>
       <c r="F70" s="16" t="n"/>
       <c r="G70" s="30" t="n"/>
-      <c r="H70" s="252" t="n"/>
       <c r="I70" s="16" t="n"/>
-      <c r="J70" s="252" t="n"/>
       <c r="K70" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -10555,9 +10453,7 @@
       <c r="E71" s="16" t="n"/>
       <c r="F71" s="16" t="n"/>
       <c r="G71" s="30" t="n"/>
-      <c r="H71" s="252" t="n"/>
       <c r="I71" s="16" t="n"/>
-      <c r="J71" s="252" t="n"/>
       <c r="K71" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -10628,9 +10524,7 @@
       <c r="E72" s="16" t="n"/>
       <c r="F72" s="16" t="n"/>
       <c r="G72" s="30" t="n"/>
-      <c r="H72" s="252" t="n"/>
       <c r="I72" s="16" t="n"/>
-      <c r="J72" s="252" t="n"/>
       <c r="K72" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -10701,7 +10595,6 @@
       <c r="E73" s="16" t="n"/>
       <c r="F73" s="16" t="n"/>
       <c r="G73" s="30" t="n"/>
-      <c r="H73" s="252" t="n"/>
       <c r="I73" s="16" t="n"/>
       <c r="J73" s="16" t="n"/>
       <c r="K73" s="16" t="n"/>
@@ -10784,9 +10677,8 @@
       <c r="E74" s="16" t="n"/>
       <c r="F74" s="16" t="n"/>
       <c r="G74" s="30" t="n"/>
-      <c r="H74" s="252" t="n"/>
       <c r="I74" s="16" t="n"/>
-      <c r="J74" s="254" t="inlineStr">
+      <c r="J74" s="253" t="inlineStr">
         <is>
           <t>Onshore Spur Line Costs ($/kW)</t>
         </is>
@@ -10877,9 +10769,7 @@
       <c r="E75" s="16" t="n"/>
       <c r="F75" s="16" t="n"/>
       <c r="G75" s="30" t="n"/>
-      <c r="H75" s="252" t="n"/>
       <c r="I75" s="16" t="n"/>
-      <c r="J75" s="252" t="n"/>
       <c r="K75" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -10954,9 +10844,7 @@
       <c r="E76" s="16" t="n"/>
       <c r="F76" s="16" t="n"/>
       <c r="G76" s="30" t="n"/>
-      <c r="H76" s="252" t="n"/>
       <c r="I76" s="16" t="n"/>
-      <c r="J76" s="252" t="n"/>
       <c r="K76" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -11049,9 +10937,7 @@
       <c r="E77" s="16" t="n"/>
       <c r="F77" s="16" t="n"/>
       <c r="G77" s="30" t="n"/>
-      <c r="H77" s="252" t="n"/>
       <c r="I77" s="16" t="n"/>
-      <c r="J77" s="252" t="n"/>
       <c r="K77" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -11122,9 +11008,7 @@
       <c r="E78" s="16" t="n"/>
       <c r="F78" s="16" t="n"/>
       <c r="G78" s="30" t="n"/>
-      <c r="H78" s="252" t="n"/>
       <c r="I78" s="16" t="n"/>
-      <c r="J78" s="252" t="n"/>
       <c r="K78" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -11333,13 +11217,13 @@
       <c r="E81" s="16" t="n"/>
       <c r="F81" s="16" t="n"/>
       <c r="G81" s="30" t="n"/>
-      <c r="H81" s="281" t="inlineStr">
+      <c r="H81" s="279" t="inlineStr">
         <is>
           <t>LCOE</t>
         </is>
       </c>
       <c r="I81" s="16" t="n"/>
-      <c r="J81" s="254" t="inlineStr">
+      <c r="J81" s="253" t="inlineStr">
         <is>
           <t>Levelized Cost of Energy ($/MWh)</t>
         </is>
@@ -11415,9 +11299,7 @@
       <c r="E82" s="16" t="n"/>
       <c r="F82" s="16" t="n"/>
       <c r="G82" s="30" t="n"/>
-      <c r="H82" s="252" t="n"/>
       <c r="I82" s="16" t="n"/>
-      <c r="J82" s="252" t="n"/>
       <c r="K82" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -11489,9 +11371,7 @@
       <c r="E83" s="16" t="n"/>
       <c r="F83" s="16" t="n"/>
       <c r="G83" s="30" t="n"/>
-      <c r="H83" s="252" t="n"/>
       <c r="I83" s="16" t="n"/>
-      <c r="J83" s="252" t="n"/>
       <c r="K83" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -11563,9 +11443,7 @@
       <c r="E84" s="16" t="n"/>
       <c r="F84" s="16" t="n"/>
       <c r="G84" s="30" t="n"/>
-      <c r="H84" s="252" t="n"/>
       <c r="I84" s="16" t="n"/>
-      <c r="J84" s="252" t="n"/>
       <c r="K84" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -11637,9 +11515,7 @@
       <c r="E85" s="16" t="n"/>
       <c r="F85" s="16" t="n"/>
       <c r="G85" s="30" t="n"/>
-      <c r="H85" s="252" t="n"/>
       <c r="I85" s="16" t="n"/>
-      <c r="J85" s="252" t="n"/>
       <c r="K85" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -11711,7 +11587,6 @@
       <c r="E86" s="16" t="n"/>
       <c r="F86" s="16" t="n"/>
       <c r="G86" s="30" t="n"/>
-      <c r="H86" s="252" t="n"/>
       <c r="I86" s="16" t="n"/>
       <c r="J86" s="16" t="n"/>
       <c r="K86" s="16" t="n"/>
@@ -11778,9 +11653,8 @@
       <c r="E87" s="16" t="n"/>
       <c r="F87" s="16" t="n"/>
       <c r="G87" s="30" t="n"/>
-      <c r="H87" s="252" t="n"/>
       <c r="I87" s="16" t="n"/>
-      <c r="J87" s="254" t="inlineStr">
+      <c r="J87" s="253" t="inlineStr">
         <is>
           <t>Overnight Levelized Cost of Energy ($/MWh)</t>
         </is>
@@ -11856,9 +11730,7 @@
       <c r="E88" s="16" t="n"/>
       <c r="F88" s="16" t="n"/>
       <c r="G88" s="30" t="n"/>
-      <c r="H88" s="252" t="n"/>
       <c r="I88" s="16" t="n"/>
-      <c r="J88" s="252" t="n"/>
       <c r="K88" s="41" t="inlineStr">
         <is>
           <t>Res PV - Chicago</t>
@@ -11930,9 +11802,7 @@
       <c r="E89" s="16" t="n"/>
       <c r="F89" s="16" t="n"/>
       <c r="G89" s="30" t="n"/>
-      <c r="H89" s="252" t="n"/>
       <c r="I89" s="16" t="n"/>
-      <c r="J89" s="252" t="n"/>
       <c r="K89" s="42" t="inlineStr">
         <is>
           <t>Res PV - Kansas City</t>
@@ -12004,9 +11874,7 @@
       <c r="E90" s="16" t="n"/>
       <c r="F90" s="16" t="n"/>
       <c r="G90" s="30" t="n"/>
-      <c r="H90" s="252" t="n"/>
       <c r="I90" s="16" t="n"/>
-      <c r="J90" s="252" t="n"/>
       <c r="K90" s="42" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles</t>
@@ -12078,9 +11946,7 @@
       <c r="E91" s="16" t="n"/>
       <c r="F91" s="16" t="n"/>
       <c r="G91" s="30" t="n"/>
-      <c r="H91" s="252" t="n"/>
       <c r="I91" s="16" t="n"/>
-      <c r="J91" s="252" t="n"/>
       <c r="K91" s="42" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA</t>
@@ -12499,19 +12365,6 @@
           <t>Future Projections</t>
         </is>
       </c>
-      <c r="H97" s="252" t="n"/>
-      <c r="I97" s="252" t="n"/>
-      <c r="J97" s="252" t="n"/>
-      <c r="K97" s="252" t="n"/>
-      <c r="L97" s="252" t="n"/>
-      <c r="M97" s="252" t="n"/>
-      <c r="N97" s="252" t="n"/>
-      <c r="O97" s="252" t="n"/>
-      <c r="P97" s="252" t="n"/>
-      <c r="Q97" s="252" t="n"/>
-      <c r="R97" s="252" t="n"/>
-      <c r="S97" s="252" t="n"/>
-      <c r="T97" s="252" t="n"/>
       <c r="U97" s="155" t="n"/>
       <c r="V97" s="155" t="n"/>
       <c r="W97" s="155" t="n"/>
@@ -12768,13 +12621,13 @@
       <c r="E100" s="16" t="n"/>
       <c r="F100" s="16" t="n"/>
       <c r="G100" s="30" t="n"/>
-      <c r="H100" s="282" t="inlineStr">
+      <c r="H100" s="280" t="inlineStr">
         <is>
           <t>Techno-Economic Cost and Performance Parameters</t>
         </is>
       </c>
       <c r="I100" s="16" t="n"/>
-      <c r="J100" s="283" t="inlineStr">
+      <c r="J100" s="281" t="inlineStr">
         <is>
           <t>Net Capacity Factor (%)</t>
         </is>
@@ -12915,9 +12768,8 @@
       <c r="E101" s="16" t="n"/>
       <c r="F101" s="16" t="n"/>
       <c r="G101" s="30" t="n"/>
-      <c r="H101" s="252" t="n"/>
       <c r="I101" s="16" t="n"/>
-      <c r="J101" s="284" t="n"/>
+      <c r="J101" s="282" t="n"/>
       <c r="K101" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -13054,9 +12906,8 @@
       <c r="E102" s="16" t="n"/>
       <c r="F102" s="16" t="n"/>
       <c r="G102" s="30" t="n"/>
-      <c r="H102" s="252" t="n"/>
       <c r="I102" s="16" t="n"/>
-      <c r="J102" s="284" t="n"/>
+      <c r="J102" s="282" t="n"/>
       <c r="K102" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -13193,9 +13044,8 @@
       <c r="E103" s="16" t="n"/>
       <c r="F103" s="16" t="n"/>
       <c r="G103" s="30" t="n"/>
-      <c r="H103" s="252" t="n"/>
       <c r="I103" s="16" t="n"/>
-      <c r="J103" s="284" t="n"/>
+      <c r="J103" s="282" t="n"/>
       <c r="K103" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -13332,9 +13182,8 @@
       <c r="E104" s="16" t="n"/>
       <c r="F104" s="16" t="n"/>
       <c r="G104" s="30" t="n"/>
-      <c r="H104" s="252" t="n"/>
       <c r="I104" s="16" t="n"/>
-      <c r="J104" s="284" t="n"/>
+      <c r="J104" s="282" t="n"/>
       <c r="K104" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -13471,9 +13320,8 @@
       <c r="E105" s="16" t="n"/>
       <c r="F105" s="16" t="n"/>
       <c r="G105" s="30" t="n"/>
-      <c r="H105" s="252" t="n"/>
       <c r="I105" s="16" t="n"/>
-      <c r="J105" s="284" t="n"/>
+      <c r="J105" s="282" t="n"/>
       <c r="K105" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -13610,9 +13458,8 @@
       <c r="E106" s="16" t="n"/>
       <c r="F106" s="16" t="n"/>
       <c r="G106" s="30" t="n"/>
-      <c r="H106" s="252" t="n"/>
       <c r="I106" s="16" t="n"/>
-      <c r="J106" s="284" t="n"/>
+      <c r="J106" s="282" t="n"/>
       <c r="K106" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -13749,9 +13596,8 @@
       <c r="E107" s="16" t="n"/>
       <c r="F107" s="16" t="n"/>
       <c r="G107" s="30" t="n"/>
-      <c r="H107" s="252" t="n"/>
       <c r="I107" s="16" t="n"/>
-      <c r="J107" s="284" t="n"/>
+      <c r="J107" s="282" t="n"/>
       <c r="K107" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -13888,9 +13734,8 @@
       <c r="E108" s="16" t="n"/>
       <c r="F108" s="16" t="n"/>
       <c r="G108" s="30" t="n"/>
-      <c r="H108" s="252" t="n"/>
       <c r="I108" s="16" t="n"/>
-      <c r="J108" s="284" t="n"/>
+      <c r="J108" s="282" t="n"/>
       <c r="K108" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -14027,9 +13872,8 @@
       <c r="E109" s="16" t="n"/>
       <c r="F109" s="16" t="n"/>
       <c r="G109" s="30" t="n"/>
-      <c r="H109" s="252" t="n"/>
       <c r="I109" s="16" t="n"/>
-      <c r="J109" s="284" t="n"/>
+      <c r="J109" s="282" t="n"/>
       <c r="K109" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -14166,9 +14010,8 @@
       <c r="E110" s="16" t="n"/>
       <c r="F110" s="16" t="n"/>
       <c r="G110" s="30" t="n"/>
-      <c r="H110" s="252" t="n"/>
       <c r="I110" s="16" t="n"/>
-      <c r="J110" s="284" t="n"/>
+      <c r="J110" s="282" t="n"/>
       <c r="K110" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -14305,9 +14148,8 @@
       <c r="E111" s="16" t="n"/>
       <c r="F111" s="16" t="n"/>
       <c r="G111" s="30" t="n"/>
-      <c r="H111" s="252" t="n"/>
       <c r="I111" s="16" t="n"/>
-      <c r="J111" s="284" t="n"/>
+      <c r="J111" s="282" t="n"/>
       <c r="K111" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -14444,9 +14286,8 @@
       <c r="E112" s="16" t="n"/>
       <c r="F112" s="16" t="n"/>
       <c r="G112" s="30" t="n"/>
-      <c r="H112" s="252" t="n"/>
       <c r="I112" s="16" t="n"/>
-      <c r="J112" s="284" t="n"/>
+      <c r="J112" s="282" t="n"/>
       <c r="K112" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -14583,9 +14424,8 @@
       <c r="E113" s="16" t="n"/>
       <c r="F113" s="16" t="n"/>
       <c r="G113" s="30" t="n"/>
-      <c r="H113" s="252" t="n"/>
       <c r="I113" s="16" t="n"/>
-      <c r="J113" s="284" t="n"/>
+      <c r="J113" s="282" t="n"/>
       <c r="K113" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -14722,9 +14562,8 @@
       <c r="E114" s="16" t="n"/>
       <c r="F114" s="16" t="n"/>
       <c r="G114" s="30" t="n"/>
-      <c r="H114" s="252" t="n"/>
       <c r="I114" s="16" t="n"/>
-      <c r="J114" s="285" t="n"/>
+      <c r="J114" s="283" t="n"/>
       <c r="K114" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -14861,7 +14700,6 @@
       <c r="E115" s="16" t="n"/>
       <c r="F115" s="16" t="n"/>
       <c r="G115" s="30" t="n"/>
-      <c r="H115" s="252" t="n"/>
       <c r="I115" s="16" t="n"/>
       <c r="J115" s="167" t="n"/>
       <c r="K115" s="19" t="n"/>
@@ -14928,7 +14766,6 @@
       <c r="E116" s="16" t="n"/>
       <c r="F116" s="16" t="n"/>
       <c r="G116" s="30" t="n"/>
-      <c r="H116" s="252" t="n"/>
       <c r="I116" s="16" t="n"/>
       <c r="J116" s="49" t="n"/>
       <c r="K116" s="16" t="n"/>
@@ -15063,9 +14900,8 @@
       <c r="E117" s="16" t="n"/>
       <c r="F117" s="16" t="n"/>
       <c r="G117" s="30" t="n"/>
-      <c r="H117" s="252" t="n"/>
       <c r="I117" s="16" t="n"/>
-      <c r="J117" s="283" t="inlineStr">
+      <c r="J117" s="281" t="inlineStr">
         <is>
           <t>Annual Energy Production (kWh/kW)</t>
         </is>
@@ -15240,9 +15076,8 @@
       <c r="E118" s="16" t="n"/>
       <c r="F118" s="16" t="n"/>
       <c r="G118" s="30" t="n"/>
-      <c r="H118" s="252" t="n"/>
       <c r="I118" s="16" t="n"/>
-      <c r="J118" s="284" t="n"/>
+      <c r="J118" s="282" t="n"/>
       <c r="K118" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -15413,9 +15248,8 @@
       <c r="E119" s="16" t="n"/>
       <c r="F119" s="16" t="n"/>
       <c r="G119" s="30" t="n"/>
-      <c r="H119" s="252" t="n"/>
       <c r="I119" s="16" t="n"/>
-      <c r="J119" s="284" t="n"/>
+      <c r="J119" s="282" t="n"/>
       <c r="K119" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -15586,9 +15420,8 @@
       <c r="E120" s="16" t="n"/>
       <c r="F120" s="16" t="n"/>
       <c r="G120" s="30" t="n"/>
-      <c r="H120" s="252" t="n"/>
       <c r="I120" s="16" t="n"/>
-      <c r="J120" s="284" t="n"/>
+      <c r="J120" s="282" t="n"/>
       <c r="K120" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -15759,9 +15592,8 @@
       <c r="E121" s="16" t="n"/>
       <c r="F121" s="16" t="n"/>
       <c r="G121" s="30" t="n"/>
-      <c r="H121" s="252" t="n"/>
       <c r="I121" s="16" t="n"/>
-      <c r="J121" s="284" t="n"/>
+      <c r="J121" s="282" t="n"/>
       <c r="K121" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -15932,9 +15764,8 @@
       <c r="E122" s="16" t="n"/>
       <c r="F122" s="16" t="n"/>
       <c r="G122" s="30" t="n"/>
-      <c r="H122" s="252" t="n"/>
       <c r="I122" s="16" t="n"/>
-      <c r="J122" s="284" t="n"/>
+      <c r="J122" s="282" t="n"/>
       <c r="K122" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -16105,9 +15936,8 @@
       <c r="E123" s="16" t="n"/>
       <c r="F123" s="16" t="n"/>
       <c r="G123" s="30" t="n"/>
-      <c r="H123" s="252" t="n"/>
       <c r="I123" s="16" t="n"/>
-      <c r="J123" s="284" t="n"/>
+      <c r="J123" s="282" t="n"/>
       <c r="K123" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -16278,9 +16108,8 @@
       <c r="E124" s="16" t="n"/>
       <c r="F124" s="16" t="n"/>
       <c r="G124" s="30" t="n"/>
-      <c r="H124" s="252" t="n"/>
       <c r="I124" s="16" t="n"/>
-      <c r="J124" s="284" t="n"/>
+      <c r="J124" s="282" t="n"/>
       <c r="K124" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -16451,9 +16280,8 @@
       <c r="E125" s="16" t="n"/>
       <c r="F125" s="16" t="n"/>
       <c r="G125" s="30" t="n"/>
-      <c r="H125" s="252" t="n"/>
       <c r="I125" s="16" t="n"/>
-      <c r="J125" s="284" t="n"/>
+      <c r="J125" s="282" t="n"/>
       <c r="K125" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -16624,9 +16452,8 @@
       <c r="E126" s="16" t="n"/>
       <c r="F126" s="16" t="n"/>
       <c r="G126" s="30" t="n"/>
-      <c r="H126" s="252" t="n"/>
       <c r="I126" s="16" t="n"/>
-      <c r="J126" s="284" t="n"/>
+      <c r="J126" s="282" t="n"/>
       <c r="K126" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -16797,9 +16624,8 @@
       <c r="E127" s="16" t="n"/>
       <c r="F127" s="16" t="n"/>
       <c r="G127" s="30" t="n"/>
-      <c r="H127" s="252" t="n"/>
       <c r="I127" s="16" t="n"/>
-      <c r="J127" s="284" t="n"/>
+      <c r="J127" s="282" t="n"/>
       <c r="K127" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -16970,9 +16796,8 @@
       <c r="E128" s="16" t="n"/>
       <c r="F128" s="16" t="n"/>
       <c r="G128" s="30" t="n"/>
-      <c r="H128" s="252" t="n"/>
       <c r="I128" s="16" t="n"/>
-      <c r="J128" s="284" t="n"/>
+      <c r="J128" s="282" t="n"/>
       <c r="K128" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -17143,9 +16968,8 @@
       <c r="E129" s="16" t="n"/>
       <c r="F129" s="16" t="n"/>
       <c r="G129" s="30" t="n"/>
-      <c r="H129" s="252" t="n"/>
       <c r="I129" s="16" t="n"/>
-      <c r="J129" s="284" t="n"/>
+      <c r="J129" s="282" t="n"/>
       <c r="K129" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -17316,9 +17140,8 @@
       <c r="E130" s="16" t="n"/>
       <c r="F130" s="16" t="n"/>
       <c r="G130" s="30" t="n"/>
-      <c r="H130" s="252" t="n"/>
       <c r="I130" s="16" t="n"/>
-      <c r="J130" s="284" t="n"/>
+      <c r="J130" s="282" t="n"/>
       <c r="K130" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -17489,9 +17312,8 @@
       <c r="E131" s="16" t="n"/>
       <c r="F131" s="16" t="n"/>
       <c r="G131" s="30" t="n"/>
-      <c r="H131" s="252" t="n"/>
       <c r="I131" s="16" t="n"/>
-      <c r="J131" s="285" t="n"/>
+      <c r="J131" s="283" t="n"/>
       <c r="K131" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -17662,7 +17484,6 @@
       <c r="E132" s="16" t="n"/>
       <c r="F132" s="16" t="n"/>
       <c r="G132" s="30" t="n"/>
-      <c r="H132" s="252" t="n"/>
       <c r="I132" s="16" t="n"/>
       <c r="J132" s="167" t="n"/>
       <c r="K132" s="19" t="n"/>
@@ -17729,7 +17550,6 @@
       <c r="E133" s="16" t="n"/>
       <c r="F133" s="16" t="n"/>
       <c r="G133" s="30" t="n"/>
-      <c r="H133" s="252" t="n"/>
       <c r="I133" s="16" t="n"/>
       <c r="J133" s="49" t="n"/>
       <c r="K133" s="16" t="n"/>
@@ -17864,9 +17684,8 @@
       <c r="E134" s="16" t="n"/>
       <c r="F134" s="16" t="n"/>
       <c r="G134" s="30" t="n"/>
-      <c r="H134" s="252" t="n"/>
       <c r="I134" s="16" t="n"/>
-      <c r="J134" s="283" t="inlineStr">
+      <c r="J134" s="281" t="inlineStr">
         <is>
           <t>CAPEX ($/kW)</t>
         </is>
@@ -18041,9 +17860,8 @@
       <c r="E135" s="16" t="n"/>
       <c r="F135" s="16" t="n"/>
       <c r="G135" s="30" t="n"/>
-      <c r="H135" s="252" t="n"/>
       <c r="I135" s="16" t="n"/>
-      <c r="J135" s="284" t="n"/>
+      <c r="J135" s="282" t="n"/>
       <c r="K135" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -18214,9 +18032,8 @@
       <c r="E136" s="16" t="n"/>
       <c r="F136" s="16" t="n"/>
       <c r="G136" s="30" t="n"/>
-      <c r="H136" s="252" t="n"/>
       <c r="I136" s="16" t="n"/>
-      <c r="J136" s="284" t="n"/>
+      <c r="J136" s="282" t="n"/>
       <c r="K136" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -18387,9 +18204,8 @@
       <c r="E137" s="16" t="n"/>
       <c r="F137" s="16" t="n"/>
       <c r="G137" s="30" t="n"/>
-      <c r="H137" s="252" t="n"/>
       <c r="I137" s="16" t="n"/>
-      <c r="J137" s="284" t="n"/>
+      <c r="J137" s="282" t="n"/>
       <c r="K137" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -18560,9 +18376,8 @@
       <c r="E138" s="16" t="n"/>
       <c r="F138" s="16" t="n"/>
       <c r="G138" s="30" t="n"/>
-      <c r="H138" s="252" t="n"/>
       <c r="I138" s="16" t="n"/>
-      <c r="J138" s="284" t="n"/>
+      <c r="J138" s="282" t="n"/>
       <c r="K138" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -18733,9 +18548,8 @@
       <c r="E139" s="16" t="n"/>
       <c r="F139" s="16" t="n"/>
       <c r="G139" s="30" t="n"/>
-      <c r="H139" s="252" t="n"/>
       <c r="I139" s="16" t="n"/>
-      <c r="J139" s="284" t="n"/>
+      <c r="J139" s="282" t="n"/>
       <c r="K139" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -18906,9 +18720,8 @@
       <c r="E140" s="16" t="n"/>
       <c r="F140" s="16" t="n"/>
       <c r="G140" s="30" t="n"/>
-      <c r="H140" s="252" t="n"/>
       <c r="I140" s="16" t="n"/>
-      <c r="J140" s="284" t="n"/>
+      <c r="J140" s="282" t="n"/>
       <c r="K140" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -19079,9 +18892,8 @@
       <c r="E141" s="16" t="n"/>
       <c r="F141" s="16" t="n"/>
       <c r="G141" s="30" t="n"/>
-      <c r="H141" s="252" t="n"/>
       <c r="I141" s="16" t="n"/>
-      <c r="J141" s="284" t="n"/>
+      <c r="J141" s="282" t="n"/>
       <c r="K141" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -19252,9 +19064,8 @@
       <c r="E142" s="16" t="n"/>
       <c r="F142" s="16" t="n"/>
       <c r="G142" s="30" t="n"/>
-      <c r="H142" s="252" t="n"/>
       <c r="I142" s="16" t="n"/>
-      <c r="J142" s="284" t="n"/>
+      <c r="J142" s="282" t="n"/>
       <c r="K142" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -19425,9 +19236,8 @@
       <c r="E143" s="16" t="n"/>
       <c r="F143" s="16" t="n"/>
       <c r="G143" s="30" t="n"/>
-      <c r="H143" s="252" t="n"/>
       <c r="I143" s="16" t="n"/>
-      <c r="J143" s="284" t="n"/>
+      <c r="J143" s="282" t="n"/>
       <c r="K143" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -19598,9 +19408,8 @@
       <c r="E144" s="16" t="n"/>
       <c r="F144" s="16" t="n"/>
       <c r="G144" s="30" t="n"/>
-      <c r="H144" s="252" t="n"/>
       <c r="I144" s="16" t="n"/>
-      <c r="J144" s="284" t="n"/>
+      <c r="J144" s="282" t="n"/>
       <c r="K144" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -19771,9 +19580,8 @@
       <c r="E145" s="16" t="n"/>
       <c r="F145" s="16" t="n"/>
       <c r="G145" s="30" t="n"/>
-      <c r="H145" s="252" t="n"/>
       <c r="I145" s="16" t="n"/>
-      <c r="J145" s="284" t="n"/>
+      <c r="J145" s="282" t="n"/>
       <c r="K145" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -19944,9 +19752,8 @@
       <c r="E146" s="16" t="n"/>
       <c r="F146" s="16" t="n"/>
       <c r="G146" s="30" t="n"/>
-      <c r="H146" s="252" t="n"/>
       <c r="I146" s="16" t="n"/>
-      <c r="J146" s="284" t="n"/>
+      <c r="J146" s="282" t="n"/>
       <c r="K146" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -20117,9 +19924,8 @@
       <c r="E147" s="16" t="n"/>
       <c r="F147" s="16" t="n"/>
       <c r="G147" s="30" t="n"/>
-      <c r="H147" s="252" t="n"/>
       <c r="I147" s="16" t="n"/>
-      <c r="J147" s="284" t="n"/>
+      <c r="J147" s="282" t="n"/>
       <c r="K147" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -20290,9 +20096,8 @@
       <c r="E148" s="16" t="n"/>
       <c r="F148" s="16" t="n"/>
       <c r="G148" s="30" t="n"/>
-      <c r="H148" s="252" t="n"/>
       <c r="I148" s="16" t="n"/>
-      <c r="J148" s="285" t="n"/>
+      <c r="J148" s="283" t="n"/>
       <c r="K148" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -20463,7 +20268,6 @@
       <c r="E149" s="16" t="n"/>
       <c r="F149" s="16" t="n"/>
       <c r="G149" s="30" t="n"/>
-      <c r="H149" s="252" t="n"/>
       <c r="I149" s="16" t="n"/>
       <c r="J149" s="167" t="n"/>
       <c r="K149" s="164" t="n"/>
@@ -20530,7 +20334,6 @@
       <c r="E150" s="16" t="n"/>
       <c r="F150" s="16" t="n"/>
       <c r="G150" s="30" t="n"/>
-      <c r="H150" s="252" t="n"/>
       <c r="I150" s="16" t="n"/>
       <c r="J150" s="16" t="n"/>
       <c r="K150" s="16" t="n"/>
@@ -20665,9 +20468,8 @@
       <c r="E151" s="16" t="n"/>
       <c r="F151" s="16" t="n"/>
       <c r="G151" s="30" t="n"/>
-      <c r="H151" s="252" t="n"/>
       <c r="I151" s="16" t="n"/>
-      <c r="J151" s="283" t="inlineStr">
+      <c r="J151" s="281" t="inlineStr">
         <is>
           <t>Overnight Capital Cost ($/kW)</t>
         </is>
@@ -20808,9 +20610,8 @@
       <c r="E152" s="16" t="n"/>
       <c r="F152" s="16" t="n"/>
       <c r="G152" s="30" t="n"/>
-      <c r="H152" s="252" t="n"/>
       <c r="I152" s="16" t="n"/>
-      <c r="J152" s="284" t="n"/>
+      <c r="J152" s="282" t="n"/>
       <c r="K152" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -20947,9 +20748,8 @@
       <c r="E153" s="16" t="n"/>
       <c r="F153" s="16" t="n"/>
       <c r="G153" s="30" t="n"/>
-      <c r="H153" s="252" t="n"/>
       <c r="I153" s="16" t="n"/>
-      <c r="J153" s="284" t="n"/>
+      <c r="J153" s="282" t="n"/>
       <c r="K153" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -21086,9 +20886,8 @@
       <c r="E154" s="16" t="n"/>
       <c r="F154" s="16" t="n"/>
       <c r="G154" s="30" t="n"/>
-      <c r="H154" s="252" t="n"/>
       <c r="I154" s="16" t="n"/>
-      <c r="J154" s="284" t="n"/>
+      <c r="J154" s="282" t="n"/>
       <c r="K154" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -21259,9 +21058,8 @@
       <c r="E155" s="16" t="n"/>
       <c r="F155" s="16" t="n"/>
       <c r="G155" s="30" t="n"/>
-      <c r="H155" s="252" t="n"/>
       <c r="I155" s="16" t="n"/>
-      <c r="J155" s="284" t="n"/>
+      <c r="J155" s="282" t="n"/>
       <c r="K155" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -21432,9 +21230,8 @@
       <c r="E156" s="16" t="n"/>
       <c r="F156" s="16" t="n"/>
       <c r="G156" s="30" t="n"/>
-      <c r="H156" s="252" t="n"/>
       <c r="I156" s="16" t="n"/>
-      <c r="J156" s="284" t="n"/>
+      <c r="J156" s="282" t="n"/>
       <c r="K156" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -21605,9 +21402,8 @@
       <c r="E157" s="16" t="n"/>
       <c r="F157" s="16" t="n"/>
       <c r="G157" s="30" t="n"/>
-      <c r="H157" s="252" t="n"/>
       <c r="I157" s="16" t="n"/>
-      <c r="J157" s="284" t="n"/>
+      <c r="J157" s="282" t="n"/>
       <c r="K157" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -21778,9 +21574,8 @@
       <c r="E158" s="16" t="n"/>
       <c r="F158" s="16" t="n"/>
       <c r="G158" s="30" t="n"/>
-      <c r="H158" s="252" t="n"/>
       <c r="I158" s="16" t="n"/>
-      <c r="J158" s="284" t="n"/>
+      <c r="J158" s="282" t="n"/>
       <c r="K158" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -21951,9 +21746,8 @@
       <c r="E159" s="16" t="n"/>
       <c r="F159" s="16" t="n"/>
       <c r="G159" s="30" t="n"/>
-      <c r="H159" s="252" t="n"/>
       <c r="I159" s="16" t="n"/>
-      <c r="J159" s="284" t="n"/>
+      <c r="J159" s="282" t="n"/>
       <c r="K159" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -22124,9 +21918,8 @@
       <c r="E160" s="16" t="n"/>
       <c r="F160" s="16" t="n"/>
       <c r="G160" s="30" t="n"/>
-      <c r="H160" s="252" t="n"/>
       <c r="I160" s="16" t="n"/>
-      <c r="J160" s="284" t="n"/>
+      <c r="J160" s="282" t="n"/>
       <c r="K160" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -22297,9 +22090,8 @@
       <c r="E161" s="16" t="n"/>
       <c r="F161" s="16" t="n"/>
       <c r="G161" s="30" t="n"/>
-      <c r="H161" s="252" t="n"/>
       <c r="I161" s="16" t="n"/>
-      <c r="J161" s="284" t="n"/>
+      <c r="J161" s="282" t="n"/>
       <c r="K161" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -22470,9 +22262,8 @@
       <c r="E162" s="16" t="n"/>
       <c r="F162" s="16" t="n"/>
       <c r="G162" s="30" t="n"/>
-      <c r="H162" s="252" t="n"/>
       <c r="I162" s="16" t="n"/>
-      <c r="J162" s="284" t="n"/>
+      <c r="J162" s="282" t="n"/>
       <c r="K162" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -22643,9 +22434,8 @@
       <c r="E163" s="16" t="n"/>
       <c r="F163" s="16" t="n"/>
       <c r="G163" s="30" t="n"/>
-      <c r="H163" s="252" t="n"/>
       <c r="I163" s="16" t="n"/>
-      <c r="J163" s="284" t="n"/>
+      <c r="J163" s="282" t="n"/>
       <c r="K163" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -22816,9 +22606,8 @@
       <c r="E164" s="16" t="n"/>
       <c r="F164" s="16" t="n"/>
       <c r="G164" s="30" t="n"/>
-      <c r="H164" s="252" t="n"/>
       <c r="I164" s="16" t="n"/>
-      <c r="J164" s="284" t="n"/>
+      <c r="J164" s="282" t="n"/>
       <c r="K164" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -22989,9 +22778,8 @@
       <c r="E165" s="16" t="n"/>
       <c r="F165" s="16" t="n"/>
       <c r="G165" s="30" t="n"/>
-      <c r="H165" s="252" t="n"/>
       <c r="I165" s="16" t="n"/>
-      <c r="J165" s="285" t="n"/>
+      <c r="J165" s="283" t="n"/>
       <c r="K165" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -23162,7 +22950,6 @@
       <c r="E166" s="16" t="n"/>
       <c r="F166" s="16" t="n"/>
       <c r="G166" s="30" t="n"/>
-      <c r="H166" s="252" t="n"/>
       <c r="I166" s="16" t="n"/>
       <c r="J166" s="167" t="n"/>
       <c r="K166" s="19" t="n"/>
@@ -23229,7 +23016,6 @@
       <c r="E167" s="16" t="n"/>
       <c r="F167" s="16" t="n"/>
       <c r="G167" s="30" t="n"/>
-      <c r="H167" s="252" t="n"/>
       <c r="I167" s="16" t="n"/>
       <c r="J167" s="16" t="n"/>
       <c r="K167" s="16" t="n"/>
@@ -23364,9 +23150,8 @@
       <c r="E168" s="16" t="n"/>
       <c r="F168" s="16" t="n"/>
       <c r="G168" s="30" t="n"/>
-      <c r="H168" s="252" t="n"/>
       <c r="I168" s="16" t="n"/>
-      <c r="J168" s="283" t="inlineStr">
+      <c r="J168" s="281" t="inlineStr">
         <is>
           <t>Fixed Operation and Maintenance Expenses ($/kW-yr)</t>
         </is>
@@ -23507,9 +23292,8 @@
       <c r="E169" s="16" t="n"/>
       <c r="F169" s="16" t="n"/>
       <c r="G169" s="30" t="n"/>
-      <c r="H169" s="252" t="n"/>
       <c r="I169" s="16" t="n"/>
-      <c r="J169" s="284" t="n"/>
+      <c r="J169" s="282" t="n"/>
       <c r="K169" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -23646,9 +23430,8 @@
       <c r="E170" s="16" t="n"/>
       <c r="F170" s="16" t="n"/>
       <c r="G170" s="30" t="n"/>
-      <c r="H170" s="252" t="n"/>
       <c r="I170" s="16" t="n"/>
-      <c r="J170" s="284" t="n"/>
+      <c r="J170" s="282" t="n"/>
       <c r="K170" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -23785,9 +23568,8 @@
       <c r="E171" s="16" t="n"/>
       <c r="F171" s="16" t="n"/>
       <c r="G171" s="30" t="n"/>
-      <c r="H171" s="252" t="n"/>
       <c r="I171" s="16" t="n"/>
-      <c r="J171" s="284" t="n"/>
+      <c r="J171" s="282" t="n"/>
       <c r="K171" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -23958,9 +23740,8 @@
       <c r="E172" s="16" t="n"/>
       <c r="F172" s="16" t="n"/>
       <c r="G172" s="30" t="n"/>
-      <c r="H172" s="252" t="n"/>
       <c r="I172" s="16" t="n"/>
-      <c r="J172" s="284" t="n"/>
+      <c r="J172" s="282" t="n"/>
       <c r="K172" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -24131,9 +23912,8 @@
       <c r="E173" s="16" t="n"/>
       <c r="F173" s="16" t="n"/>
       <c r="G173" s="30" t="n"/>
-      <c r="H173" s="252" t="n"/>
       <c r="I173" s="16" t="n"/>
-      <c r="J173" s="284" t="n"/>
+      <c r="J173" s="282" t="n"/>
       <c r="K173" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -24304,9 +24084,8 @@
       <c r="E174" s="16" t="n"/>
       <c r="F174" s="16" t="n"/>
       <c r="G174" s="30" t="n"/>
-      <c r="H174" s="252" t="n"/>
       <c r="I174" s="16" t="n"/>
-      <c r="J174" s="284" t="n"/>
+      <c r="J174" s="282" t="n"/>
       <c r="K174" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -24477,9 +24256,8 @@
       <c r="E175" s="16" t="n"/>
       <c r="F175" s="16" t="n"/>
       <c r="G175" s="30" t="n"/>
-      <c r="H175" s="252" t="n"/>
       <c r="I175" s="16" t="n"/>
-      <c r="J175" s="284" t="n"/>
+      <c r="J175" s="282" t="n"/>
       <c r="K175" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -24650,9 +24428,8 @@
       <c r="E176" s="16" t="n"/>
       <c r="F176" s="16" t="n"/>
       <c r="G176" s="30" t="n"/>
-      <c r="H176" s="252" t="n"/>
       <c r="I176" s="16" t="n"/>
-      <c r="J176" s="284" t="n"/>
+      <c r="J176" s="282" t="n"/>
       <c r="K176" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -24823,9 +24600,8 @@
       <c r="E177" s="16" t="n"/>
       <c r="F177" s="16" t="n"/>
       <c r="G177" s="30" t="n"/>
-      <c r="H177" s="252" t="n"/>
       <c r="I177" s="16" t="n"/>
-      <c r="J177" s="284" t="n"/>
+      <c r="J177" s="282" t="n"/>
       <c r="K177" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -24996,9 +24772,8 @@
       <c r="E178" s="16" t="n"/>
       <c r="F178" s="16" t="n"/>
       <c r="G178" s="30" t="n"/>
-      <c r="H178" s="252" t="n"/>
       <c r="I178" s="16" t="n"/>
-      <c r="J178" s="284" t="n"/>
+      <c r="J178" s="282" t="n"/>
       <c r="K178" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -25169,9 +24944,8 @@
       <c r="E179" s="16" t="n"/>
       <c r="F179" s="16" t="n"/>
       <c r="G179" s="30" t="n"/>
-      <c r="H179" s="252" t="n"/>
       <c r="I179" s="16" t="n"/>
-      <c r="J179" s="284" t="n"/>
+      <c r="J179" s="282" t="n"/>
       <c r="K179" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -25342,9 +25116,8 @@
       <c r="E180" s="16" t="n"/>
       <c r="F180" s="16" t="n"/>
       <c r="G180" s="30" t="n"/>
-      <c r="H180" s="252" t="n"/>
       <c r="I180" s="16" t="n"/>
-      <c r="J180" s="284" t="n"/>
+      <c r="J180" s="282" t="n"/>
       <c r="K180" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -25515,9 +25288,8 @@
       <c r="E181" s="16" t="n"/>
       <c r="F181" s="16" t="n"/>
       <c r="G181" s="30" t="n"/>
-      <c r="H181" s="252" t="n"/>
       <c r="I181" s="16" t="n"/>
-      <c r="J181" s="284" t="n"/>
+      <c r="J181" s="282" t="n"/>
       <c r="K181" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -25688,9 +25460,8 @@
       <c r="E182" s="16" t="n"/>
       <c r="F182" s="16" t="n"/>
       <c r="G182" s="30" t="n"/>
-      <c r="H182" s="252" t="n"/>
       <c r="I182" s="16" t="n"/>
-      <c r="J182" s="285" t="n"/>
+      <c r="J182" s="283" t="n"/>
       <c r="K182" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -25861,7 +25632,6 @@
       <c r="E183" s="16" t="n"/>
       <c r="F183" s="16" t="n"/>
       <c r="G183" s="30" t="n"/>
-      <c r="H183" s="252" t="n"/>
       <c r="I183" s="16" t="n"/>
       <c r="J183" s="167" t="n"/>
       <c r="K183" s="19" t="n"/>
@@ -25928,7 +25698,6 @@
       <c r="E184" s="16" t="n"/>
       <c r="F184" s="16" t="n"/>
       <c r="G184" s="30" t="n"/>
-      <c r="H184" s="252" t="n"/>
       <c r="I184" s="16" t="n"/>
       <c r="J184" s="16" t="n"/>
       <c r="K184" s="16" t="n"/>
@@ -26063,9 +25832,8 @@
       <c r="E185" s="16" t="n"/>
       <c r="F185" s="16" t="n"/>
       <c r="G185" s="30" t="n"/>
-      <c r="H185" s="252" t="n"/>
       <c r="I185" s="16" t="n"/>
-      <c r="J185" s="283" t="inlineStr">
+      <c r="J185" s="281" t="inlineStr">
         <is>
           <t>Variable Operation and Maintenance Expenses ($/MWh)</t>
         </is>
@@ -26206,9 +25974,8 @@
       <c r="E186" s="16" t="n"/>
       <c r="F186" s="16" t="n"/>
       <c r="G186" s="30" t="n"/>
-      <c r="H186" s="252" t="n"/>
       <c r="I186" s="16" t="n"/>
-      <c r="J186" s="284" t="n"/>
+      <c r="J186" s="282" t="n"/>
       <c r="K186" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -26345,9 +26112,8 @@
       <c r="E187" s="16" t="n"/>
       <c r="F187" s="16" t="n"/>
       <c r="G187" s="30" t="n"/>
-      <c r="H187" s="252" t="n"/>
       <c r="I187" s="16" t="n"/>
-      <c r="J187" s="284" t="n"/>
+      <c r="J187" s="282" t="n"/>
       <c r="K187" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -26484,9 +26250,8 @@
       <c r="E188" s="16" t="n"/>
       <c r="F188" s="16" t="n"/>
       <c r="G188" s="30" t="n"/>
-      <c r="H188" s="252" t="n"/>
       <c r="I188" s="16" t="n"/>
-      <c r="J188" s="284" t="n"/>
+      <c r="J188" s="282" t="n"/>
       <c r="K188" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -26623,9 +26388,8 @@
       <c r="E189" s="16" t="n"/>
       <c r="F189" s="16" t="n"/>
       <c r="G189" s="30" t="n"/>
-      <c r="H189" s="252" t="n"/>
       <c r="I189" s="16" t="n"/>
-      <c r="J189" s="284" t="n"/>
+      <c r="J189" s="282" t="n"/>
       <c r="K189" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -26762,9 +26526,8 @@
       <c r="E190" s="16" t="n"/>
       <c r="F190" s="16" t="n"/>
       <c r="G190" s="30" t="n"/>
-      <c r="H190" s="252" t="n"/>
       <c r="I190" s="16" t="n"/>
-      <c r="J190" s="284" t="n"/>
+      <c r="J190" s="282" t="n"/>
       <c r="K190" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -26901,9 +26664,8 @@
       <c r="E191" s="16" t="n"/>
       <c r="F191" s="16" t="n"/>
       <c r="G191" s="30" t="n"/>
-      <c r="H191" s="252" t="n"/>
       <c r="I191" s="16" t="n"/>
-      <c r="J191" s="284" t="n"/>
+      <c r="J191" s="282" t="n"/>
       <c r="K191" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -27040,9 +26802,8 @@
       <c r="E192" s="16" t="n"/>
       <c r="F192" s="16" t="n"/>
       <c r="G192" s="30" t="n"/>
-      <c r="H192" s="252" t="n"/>
       <c r="I192" s="16" t="n"/>
-      <c r="J192" s="284" t="n"/>
+      <c r="J192" s="282" t="n"/>
       <c r="K192" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -27183,9 +26944,8 @@
       <c r="E193" s="16" t="n"/>
       <c r="F193" s="16" t="n"/>
       <c r="G193" s="30" t="n"/>
-      <c r="H193" s="252" t="n"/>
       <c r="I193" s="16" t="n"/>
-      <c r="J193" s="284" t="n"/>
+      <c r="J193" s="282" t="n"/>
       <c r="K193" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -27322,9 +27082,8 @@
       <c r="E194" s="16" t="n"/>
       <c r="F194" s="16" t="n"/>
       <c r="G194" s="30" t="n"/>
-      <c r="H194" s="252" t="n"/>
       <c r="I194" s="16" t="n"/>
-      <c r="J194" s="284" t="n"/>
+      <c r="J194" s="282" t="n"/>
       <c r="K194" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -27461,9 +27220,8 @@
       <c r="E195" s="16" t="n"/>
       <c r="F195" s="16" t="n"/>
       <c r="G195" s="30" t="n"/>
-      <c r="H195" s="252" t="n"/>
       <c r="I195" s="16" t="n"/>
-      <c r="J195" s="284" t="n"/>
+      <c r="J195" s="282" t="n"/>
       <c r="K195" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -27604,9 +27362,8 @@
       <c r="E196" s="16" t="n"/>
       <c r="F196" s="16" t="n"/>
       <c r="G196" s="30" t="n"/>
-      <c r="H196" s="252" t="n"/>
       <c r="I196" s="16" t="n"/>
-      <c r="J196" s="284" t="n"/>
+      <c r="J196" s="282" t="n"/>
       <c r="K196" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -27743,9 +27500,8 @@
       <c r="E197" s="16" t="n"/>
       <c r="F197" s="16" t="n"/>
       <c r="G197" s="30" t="n"/>
-      <c r="H197" s="252" t="n"/>
       <c r="I197" s="16" t="n"/>
-      <c r="J197" s="284" t="n"/>
+      <c r="J197" s="282" t="n"/>
       <c r="K197" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -27882,9 +27638,8 @@
       <c r="E198" s="16" t="n"/>
       <c r="F198" s="16" t="n"/>
       <c r="G198" s="30" t="n"/>
-      <c r="H198" s="252" t="n"/>
       <c r="I198" s="16" t="n"/>
-      <c r="J198" s="284" t="n"/>
+      <c r="J198" s="282" t="n"/>
       <c r="K198" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -28025,9 +27780,8 @@
       <c r="E199" s="16" t="n"/>
       <c r="F199" s="16" t="n"/>
       <c r="G199" s="30" t="n"/>
-      <c r="H199" s="252" t="n"/>
       <c r="I199" s="16" t="n"/>
-      <c r="J199" s="285" t="n"/>
+      <c r="J199" s="283" t="n"/>
       <c r="K199" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -28433,7 +28187,7 @@
       <c r="E203" s="16" t="n"/>
       <c r="F203" s="16" t="n"/>
       <c r="G203" s="16" t="n"/>
-      <c r="H203" s="278" t="inlineStr">
+      <c r="H203" s="276" t="inlineStr">
         <is>
           <t>Finance</t>
         </is>
@@ -28580,9 +28334,7 @@
       <c r="E204" s="16" t="n"/>
       <c r="F204" s="16" t="n"/>
       <c r="G204" s="16" t="n"/>
-      <c r="H204" s="252" t="n"/>
       <c r="I204" s="16" t="n"/>
-      <c r="J204" s="252" t="n"/>
       <c r="K204" s="196" t="inlineStr">
         <is>
           <t>Interest Rate Nominal - Low</t>
@@ -28719,9 +28471,7 @@
       <c r="E205" s="16" t="n"/>
       <c r="F205" s="16" t="n"/>
       <c r="G205" s="16" t="n"/>
-      <c r="H205" s="252" t="n"/>
       <c r="I205" s="16" t="n"/>
-      <c r="J205" s="252" t="n"/>
       <c r="K205" s="196" t="inlineStr">
         <is>
           <t>Interest Rate Nominal - Mid</t>
@@ -28858,9 +28608,7 @@
       <c r="E206" s="16" t="n"/>
       <c r="F206" s="16" t="n"/>
       <c r="G206" s="16" t="n"/>
-      <c r="H206" s="252" t="n"/>
       <c r="I206" s="16" t="n"/>
-      <c r="J206" s="252" t="n"/>
       <c r="K206" s="196" t="inlineStr">
         <is>
           <t>Interest Rate Nominal - Constant</t>
@@ -28997,9 +28745,7 @@
       <c r="E207" s="16" t="n"/>
       <c r="F207" s="16" t="n"/>
       <c r="G207" s="16" t="n"/>
-      <c r="H207" s="252" t="n"/>
       <c r="I207" s="16" t="n"/>
-      <c r="J207" s="252" t="n"/>
       <c r="K207" s="196" t="inlineStr">
         <is>
           <t>Calculated Interest Rate Real - Low</t>
@@ -29136,9 +28882,7 @@
       <c r="E208" s="16" t="n"/>
       <c r="F208" s="16" t="n"/>
       <c r="G208" s="16" t="n"/>
-      <c r="H208" s="252" t="n"/>
       <c r="I208" s="16" t="n"/>
-      <c r="J208" s="252" t="n"/>
       <c r="K208" s="196" t="inlineStr">
         <is>
           <t>Calculated Interest Rate Real - Mid</t>
@@ -29275,9 +29019,7 @@
       <c r="E209" s="16" t="n"/>
       <c r="F209" s="16" t="n"/>
       <c r="G209" s="16" t="n"/>
-      <c r="H209" s="252" t="n"/>
       <c r="I209" s="16" t="n"/>
-      <c r="J209" s="252" t="n"/>
       <c r="K209" s="196" t="inlineStr">
         <is>
           <t>Calculated Interest Rate Real - Constant</t>
@@ -29414,9 +29156,7 @@
       <c r="E210" s="16" t="n"/>
       <c r="F210" s="16" t="n"/>
       <c r="G210" s="16" t="n"/>
-      <c r="H210" s="252" t="n"/>
       <c r="I210" s="16" t="n"/>
-      <c r="J210" s="252" t="n"/>
       <c r="K210" s="196" t="inlineStr">
         <is>
           <t>Interest During Construction  - Nominal</t>
@@ -29553,9 +29293,7 @@
       <c r="E211" s="16" t="n"/>
       <c r="F211" s="16" t="n"/>
       <c r="G211" s="16" t="n"/>
-      <c r="H211" s="252" t="n"/>
       <c r="I211" s="16" t="n"/>
-      <c r="J211" s="252" t="n"/>
       <c r="K211" s="196" t="inlineStr">
         <is>
           <t>Rate of Return on Equity Nominal - Low</t>
@@ -29692,9 +29430,7 @@
       <c r="E212" s="16" t="n"/>
       <c r="F212" s="16" t="n"/>
       <c r="G212" s="16" t="n"/>
-      <c r="H212" s="252" t="n"/>
       <c r="I212" s="16" t="n"/>
-      <c r="J212" s="252" t="n"/>
       <c r="K212" s="196" t="inlineStr">
         <is>
           <t>Rate of Return on Equity Nominal - Mid</t>
@@ -29831,9 +29567,7 @@
       <c r="E213" s="16" t="n"/>
       <c r="F213" s="16" t="n"/>
       <c r="G213" s="16" t="n"/>
-      <c r="H213" s="252" t="n"/>
       <c r="I213" s="16" t="n"/>
-      <c r="J213" s="252" t="n"/>
       <c r="K213" s="196" t="inlineStr">
         <is>
           <t>Rate of Return on Equity Nominal - Constant</t>
@@ -29970,9 +29704,7 @@
       <c r="E214" s="16" t="n"/>
       <c r="F214" s="16" t="n"/>
       <c r="G214" s="16" t="n"/>
-      <c r="H214" s="252" t="n"/>
       <c r="I214" s="16" t="n"/>
-      <c r="J214" s="252" t="n"/>
       <c r="K214" s="196" t="inlineStr">
         <is>
           <t>Calculated Rate of Return on Equity Real - Low</t>
@@ -30109,9 +29841,7 @@
       <c r="E215" s="16" t="n"/>
       <c r="F215" s="16" t="n"/>
       <c r="G215" s="16" t="n"/>
-      <c r="H215" s="252" t="n"/>
       <c r="I215" s="16" t="n"/>
-      <c r="J215" s="252" t="n"/>
       <c r="K215" s="196" t="inlineStr">
         <is>
           <t>Calculated Rate of Return on Equity Real - Mid</t>
@@ -30248,9 +29978,7 @@
       <c r="E216" s="16" t="n"/>
       <c r="F216" s="16" t="n"/>
       <c r="G216" s="16" t="n"/>
-      <c r="H216" s="252" t="n"/>
       <c r="I216" s="16" t="n"/>
-      <c r="J216" s="252" t="n"/>
       <c r="K216" s="196" t="inlineStr">
         <is>
           <t>Calculated Rate of Return on Equity Real - Constant</t>
@@ -30387,9 +30115,7 @@
       <c r="E217" s="16" t="n"/>
       <c r="F217" s="16" t="n"/>
       <c r="G217" s="16" t="n"/>
-      <c r="H217" s="252" t="n"/>
       <c r="I217" s="16" t="n"/>
-      <c r="J217" s="252" t="n"/>
       <c r="K217" s="196" t="inlineStr">
         <is>
           <t>Debt Fraction - Low</t>
@@ -30526,9 +30252,7 @@
       <c r="E218" s="16" t="n"/>
       <c r="F218" s="16" t="n"/>
       <c r="G218" s="16" t="n"/>
-      <c r="H218" s="252" t="n"/>
       <c r="I218" s="16" t="n"/>
-      <c r="J218" s="252" t="n"/>
       <c r="K218" s="196" t="inlineStr">
         <is>
           <t>Debt Fraction - Mid</t>
@@ -30665,9 +30389,7 @@
       <c r="E219" s="16" t="n"/>
       <c r="F219" s="16" t="n"/>
       <c r="G219" s="16" t="n"/>
-      <c r="H219" s="252" t="n"/>
       <c r="I219" s="16" t="n"/>
-      <c r="J219" s="252" t="n"/>
       <c r="K219" s="196" t="inlineStr">
         <is>
           <t>Debt Fraction - Constant</t>
@@ -30804,9 +30526,7 @@
       <c r="E220" s="16" t="n"/>
       <c r="F220" s="16" t="n"/>
       <c r="G220" s="16" t="n"/>
-      <c r="H220" s="252" t="n"/>
       <c r="I220" s="16" t="n"/>
-      <c r="J220" s="252" t="n"/>
       <c r="K220" s="196" t="inlineStr">
         <is>
           <t>Tax Rate (Federal and State)</t>
@@ -30943,9 +30663,7 @@
       <c r="E221" s="16" t="n"/>
       <c r="F221" s="16" t="n"/>
       <c r="G221" s="16" t="n"/>
-      <c r="H221" s="252" t="n"/>
       <c r="I221" s="16" t="n"/>
-      <c r="J221" s="252" t="n"/>
       <c r="K221" s="196" t="inlineStr">
         <is>
           <t>WACC Nominal - Low</t>
@@ -31082,9 +30800,7 @@
       <c r="E222" s="16" t="n"/>
       <c r="F222" s="16" t="n"/>
       <c r="G222" s="16" t="n"/>
-      <c r="H222" s="252" t="n"/>
       <c r="I222" s="16" t="n"/>
-      <c r="J222" s="252" t="n"/>
       <c r="K222" s="196" t="inlineStr">
         <is>
           <t>WACC Nominal - Mid</t>
@@ -31221,9 +30937,7 @@
       <c r="E223" s="16" t="n"/>
       <c r="F223" s="16" t="n"/>
       <c r="G223" s="16" t="n"/>
-      <c r="H223" s="252" t="n"/>
       <c r="I223" s="16" t="n"/>
-      <c r="J223" s="252" t="n"/>
       <c r="K223" s="196" t="inlineStr">
         <is>
           <t>WACC Nominal - Constant</t>
@@ -31360,9 +31074,7 @@
       <c r="E224" s="16" t="n"/>
       <c r="F224" s="16" t="n"/>
       <c r="G224" s="16" t="n"/>
-      <c r="H224" s="252" t="n"/>
       <c r="I224" s="16" t="n"/>
-      <c r="J224" s="252" t="n"/>
       <c r="K224" s="196" t="inlineStr">
         <is>
           <t>WACC Real - Low</t>
@@ -31499,9 +31211,7 @@
       <c r="E225" s="16" t="n"/>
       <c r="F225" s="16" t="n"/>
       <c r="G225" s="16" t="n"/>
-      <c r="H225" s="252" t="n"/>
       <c r="I225" s="16" t="n"/>
-      <c r="J225" s="252" t="n"/>
       <c r="K225" s="196" t="inlineStr">
         <is>
           <t>WACC Real - Mid</t>
@@ -31638,9 +31348,7 @@
       <c r="E226" s="16" t="n"/>
       <c r="F226" s="16" t="n"/>
       <c r="G226" s="16" t="n"/>
-      <c r="H226" s="252" t="n"/>
       <c r="I226" s="16" t="n"/>
-      <c r="J226" s="252" t="n"/>
       <c r="K226" s="196" t="inlineStr">
         <is>
           <t>WACC Real - Constant</t>
@@ -31777,9 +31485,7 @@
       <c r="E227" s="16" t="n"/>
       <c r="F227" s="16" t="n"/>
       <c r="G227" s="16" t="n"/>
-      <c r="H227" s="252" t="n"/>
       <c r="I227" s="16" t="n"/>
-      <c r="J227" s="252" t="n"/>
       <c r="K227" s="198" t="inlineStr">
         <is>
           <t>Capital Recovery Factor (CRF) Nominal - Low</t>
@@ -31950,9 +31656,7 @@
       <c r="E228" s="16" t="n"/>
       <c r="F228" s="16" t="n"/>
       <c r="G228" s="16" t="n"/>
-      <c r="H228" s="252" t="n"/>
       <c r="I228" s="16" t="n"/>
-      <c r="J228" s="252" t="n"/>
       <c r="K228" s="198" t="inlineStr">
         <is>
           <t>Capital Recovery Factor (CRF) Nominal - Mid</t>
@@ -32123,9 +31827,7 @@
       <c r="E229" s="16" t="n"/>
       <c r="F229" s="16" t="n"/>
       <c r="G229" s="16" t="n"/>
-      <c r="H229" s="252" t="n"/>
       <c r="I229" s="16" t="n"/>
-      <c r="J229" s="252" t="n"/>
       <c r="K229" s="198" t="inlineStr">
         <is>
           <t>Capital Recovery Factor (CRF) Nominal - Constant</t>
@@ -32296,9 +31998,7 @@
       <c r="E230" s="16" t="n"/>
       <c r="F230" s="16" t="n"/>
       <c r="G230" s="16" t="n"/>
-      <c r="H230" s="252" t="n"/>
       <c r="I230" s="16" t="n"/>
-      <c r="J230" s="252" t="n"/>
       <c r="K230" s="198" t="inlineStr">
         <is>
           <t>Capital Recovery Factor (CRF) Real - Low</t>
@@ -32469,7 +32169,6 @@
       <c r="E231" s="16" t="n"/>
       <c r="F231" s="16" t="n"/>
       <c r="G231" s="16" t="n"/>
-      <c r="H231" s="252" t="n"/>
       <c r="I231" s="16" t="n"/>
       <c r="J231" s="199" t="n"/>
       <c r="K231" s="198" t="inlineStr">
@@ -32642,7 +32341,6 @@
       <c r="E232" s="16" t="n"/>
       <c r="F232" s="16" t="n"/>
       <c r="G232" s="16" t="n"/>
-      <c r="H232" s="252" t="n"/>
       <c r="I232" s="16" t="n"/>
       <c r="J232" s="199" t="n"/>
       <c r="K232" s="198" t="inlineStr">
@@ -32815,7 +32513,6 @@
       <c r="E233" s="16" t="n"/>
       <c r="F233" s="16" t="n"/>
       <c r="G233" s="16" t="n"/>
-      <c r="H233" s="252" t="n"/>
       <c r="I233" s="16" t="n"/>
       <c r="J233" s="16" t="n"/>
       <c r="K233" s="16" t="n"/>
@@ -32882,7 +32579,6 @@
       <c r="E234" s="16" t="n"/>
       <c r="F234" s="16" t="n"/>
       <c r="G234" s="30" t="n"/>
-      <c r="H234" s="252" t="n"/>
       <c r="I234" s="16" t="n"/>
       <c r="J234" s="16" t="n"/>
       <c r="K234" s="16" t="n"/>
@@ -33017,9 +32713,8 @@
       <c r="E235" s="16" t="n"/>
       <c r="F235" s="16" t="n"/>
       <c r="G235" s="30" t="n"/>
-      <c r="H235" s="252" t="n"/>
       <c r="I235" s="16" t="n"/>
-      <c r="J235" s="283" t="inlineStr">
+      <c r="J235" s="281" t="inlineStr">
         <is>
           <t>Weighted Average Cost of Capital (WACC) (Nominal) (%)</t>
         </is>
@@ -33194,9 +32889,8 @@
       <c r="E236" s="16" t="n"/>
       <c r="F236" s="16" t="n"/>
       <c r="G236" s="30" t="n"/>
-      <c r="H236" s="252" t="n"/>
       <c r="I236" s="16" t="n"/>
-      <c r="J236" s="284" t="n"/>
+      <c r="J236" s="282" t="n"/>
       <c r="K236" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -33367,9 +33061,8 @@
       <c r="E237" s="16" t="n"/>
       <c r="F237" s="16" t="n"/>
       <c r="G237" s="30" t="n"/>
-      <c r="H237" s="252" t="n"/>
       <c r="I237" s="16" t="n"/>
-      <c r="J237" s="284" t="n"/>
+      <c r="J237" s="282" t="n"/>
       <c r="K237" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -33540,9 +33233,8 @@
       <c r="E238" s="16" t="n"/>
       <c r="F238" s="16" t="n"/>
       <c r="G238" s="30" t="n"/>
-      <c r="H238" s="252" t="n"/>
       <c r="I238" s="16" t="n"/>
-      <c r="J238" s="284" t="n"/>
+      <c r="J238" s="282" t="n"/>
       <c r="K238" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -33713,9 +33405,8 @@
       <c r="E239" s="16" t="n"/>
       <c r="F239" s="16" t="n"/>
       <c r="G239" s="30" t="n"/>
-      <c r="H239" s="252" t="n"/>
       <c r="I239" s="16" t="n"/>
-      <c r="J239" s="284" t="n"/>
+      <c r="J239" s="282" t="n"/>
       <c r="K239" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -33886,9 +33577,8 @@
       <c r="E240" s="16" t="n"/>
       <c r="F240" s="16" t="n"/>
       <c r="G240" s="30" t="n"/>
-      <c r="H240" s="252" t="n"/>
       <c r="I240" s="16" t="n"/>
-      <c r="J240" s="284" t="n"/>
+      <c r="J240" s="282" t="n"/>
       <c r="K240" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -34059,9 +33749,8 @@
       <c r="E241" s="16" t="n"/>
       <c r="F241" s="16" t="n"/>
       <c r="G241" s="30" t="n"/>
-      <c r="H241" s="252" t="n"/>
       <c r="I241" s="97" t="n"/>
-      <c r="J241" s="284" t="n"/>
+      <c r="J241" s="282" t="n"/>
       <c r="K241" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -34232,9 +33921,8 @@
       <c r="E242" s="16" t="n"/>
       <c r="F242" s="16" t="n"/>
       <c r="G242" s="30" t="n"/>
-      <c r="H242" s="252" t="n"/>
       <c r="I242" s="101" t="n"/>
-      <c r="J242" s="284" t="n"/>
+      <c r="J242" s="282" t="n"/>
       <c r="K242" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -34405,9 +34093,8 @@
       <c r="E243" s="16" t="n"/>
       <c r="F243" s="16" t="n"/>
       <c r="G243" s="30" t="n"/>
-      <c r="H243" s="252" t="n"/>
       <c r="I243" s="16" t="n"/>
-      <c r="J243" s="284" t="n"/>
+      <c r="J243" s="282" t="n"/>
       <c r="K243" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -34578,9 +34265,8 @@
       <c r="E244" s="16" t="n"/>
       <c r="F244" s="16" t="n"/>
       <c r="G244" s="30" t="n"/>
-      <c r="H244" s="252" t="n"/>
       <c r="I244" s="97" t="n"/>
-      <c r="J244" s="284" t="n"/>
+      <c r="J244" s="282" t="n"/>
       <c r="K244" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -34751,9 +34437,8 @@
       <c r="E245" s="16" t="n"/>
       <c r="F245" s="16" t="n"/>
       <c r="G245" s="30" t="n"/>
-      <c r="H245" s="252" t="n"/>
       <c r="I245" s="101" t="n"/>
-      <c r="J245" s="284" t="n"/>
+      <c r="J245" s="282" t="n"/>
       <c r="K245" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -34924,9 +34609,8 @@
       <c r="E246" s="16" t="n"/>
       <c r="F246" s="16" t="n"/>
       <c r="G246" s="30" t="n"/>
-      <c r="H246" s="252" t="n"/>
       <c r="I246" s="16" t="n"/>
-      <c r="J246" s="284" t="n"/>
+      <c r="J246" s="282" t="n"/>
       <c r="K246" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -35097,9 +34781,8 @@
       <c r="E247" s="16" t="n"/>
       <c r="F247" s="16" t="n"/>
       <c r="G247" s="30" t="n"/>
-      <c r="H247" s="252" t="n"/>
       <c r="I247" s="97" t="n"/>
-      <c r="J247" s="284" t="n"/>
+      <c r="J247" s="282" t="n"/>
       <c r="K247" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -35270,9 +34953,8 @@
       <c r="E248" s="16" t="n"/>
       <c r="F248" s="16" t="n"/>
       <c r="G248" s="30" t="n"/>
-      <c r="H248" s="252" t="n"/>
       <c r="I248" s="101" t="n"/>
-      <c r="J248" s="284" t="n"/>
+      <c r="J248" s="282" t="n"/>
       <c r="K248" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -35443,9 +35125,8 @@
       <c r="E249" s="16" t="n"/>
       <c r="F249" s="16" t="n"/>
       <c r="G249" s="30" t="n"/>
-      <c r="H249" s="252" t="n"/>
       <c r="I249" s="16" t="n"/>
-      <c r="J249" s="285" t="n"/>
+      <c r="J249" s="283" t="n"/>
       <c r="K249" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -35818,13 +35499,13 @@
       <c r="E252" s="16" t="n"/>
       <c r="F252" s="16" t="n"/>
       <c r="G252" s="30" t="n"/>
-      <c r="H252" s="280" t="inlineStr">
+      <c r="H252" s="278" t="inlineStr">
         <is>
           <t>Grid Connection Costs</t>
         </is>
       </c>
       <c r="I252" s="16" t="n"/>
-      <c r="J252" s="283" t="inlineStr">
+      <c r="J252" s="281" t="inlineStr">
         <is>
           <t>Grid Connection Costs (GCC) ($/kW)</t>
         </is>
@@ -35965,9 +35646,8 @@
       <c r="E253" s="16" t="n"/>
       <c r="F253" s="16" t="n"/>
       <c r="G253" s="30" t="n"/>
-      <c r="H253" s="252" t="n"/>
       <c r="I253" s="16" t="n"/>
-      <c r="J253" s="284" t="n"/>
+      <c r="J253" s="282" t="n"/>
       <c r="K253" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -36104,9 +35784,8 @@
       <c r="E254" s="16" t="n"/>
       <c r="F254" s="16" t="n"/>
       <c r="G254" s="30" t="n"/>
-      <c r="H254" s="252" t="n"/>
       <c r="I254" s="16" t="n"/>
-      <c r="J254" s="284" t="n"/>
+      <c r="J254" s="282" t="n"/>
       <c r="K254" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -36243,9 +35922,8 @@
       <c r="E255" s="16" t="n"/>
       <c r="F255" s="16" t="n"/>
       <c r="G255" s="30" t="n"/>
-      <c r="H255" s="252" t="n"/>
       <c r="I255" s="16" t="n"/>
-      <c r="J255" s="284" t="n"/>
+      <c r="J255" s="282" t="n"/>
       <c r="K255" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -36382,9 +36060,8 @@
       <c r="E256" s="16" t="n"/>
       <c r="F256" s="16" t="n"/>
       <c r="G256" s="30" t="n"/>
-      <c r="H256" s="252" t="n"/>
       <c r="I256" s="16" t="n"/>
-      <c r="J256" s="284" t="n"/>
+      <c r="J256" s="282" t="n"/>
       <c r="K256" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -36521,9 +36198,8 @@
       <c r="E257" s="16" t="n"/>
       <c r="F257" s="16" t="n"/>
       <c r="G257" s="30" t="n"/>
-      <c r="H257" s="252" t="n"/>
       <c r="I257" s="16" t="n"/>
-      <c r="J257" s="284" t="n"/>
+      <c r="J257" s="282" t="n"/>
       <c r="K257" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -36660,9 +36336,8 @@
       <c r="E258" s="16" t="n"/>
       <c r="F258" s="16" t="n"/>
       <c r="G258" s="30" t="n"/>
-      <c r="H258" s="252" t="n"/>
       <c r="I258" s="16" t="n"/>
-      <c r="J258" s="284" t="n"/>
+      <c r="J258" s="282" t="n"/>
       <c r="K258" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -36799,9 +36474,8 @@
       <c r="E259" s="16" t="n"/>
       <c r="F259" s="16" t="n"/>
       <c r="G259" s="30" t="n"/>
-      <c r="H259" s="252" t="n"/>
       <c r="I259" s="16" t="n"/>
-      <c r="J259" s="284" t="n"/>
+      <c r="J259" s="282" t="n"/>
       <c r="K259" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -36938,9 +36612,8 @@
       <c r="E260" s="16" t="n"/>
       <c r="F260" s="16" t="n"/>
       <c r="G260" s="30" t="n"/>
-      <c r="H260" s="252" t="n"/>
       <c r="I260" s="16" t="n"/>
-      <c r="J260" s="284" t="n"/>
+      <c r="J260" s="282" t="n"/>
       <c r="K260" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -37077,9 +36750,8 @@
       <c r="E261" s="16" t="n"/>
       <c r="F261" s="16" t="n"/>
       <c r="G261" s="30" t="n"/>
-      <c r="H261" s="252" t="n"/>
       <c r="I261" s="16" t="n"/>
-      <c r="J261" s="284" t="n"/>
+      <c r="J261" s="282" t="n"/>
       <c r="K261" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -37216,9 +36888,8 @@
       <c r="E262" s="16" t="n"/>
       <c r="F262" s="16" t="n"/>
       <c r="G262" s="30" t="n"/>
-      <c r="H262" s="252" t="n"/>
       <c r="I262" s="16" t="n"/>
-      <c r="J262" s="284" t="n"/>
+      <c r="J262" s="282" t="n"/>
       <c r="K262" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -37355,9 +37026,8 @@
       <c r="E263" s="16" t="n"/>
       <c r="F263" s="16" t="n"/>
       <c r="G263" s="30" t="n"/>
-      <c r="H263" s="252" t="n"/>
       <c r="I263" s="16" t="n"/>
-      <c r="J263" s="284" t="n"/>
+      <c r="J263" s="282" t="n"/>
       <c r="K263" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -37494,9 +37164,8 @@
       <c r="E264" s="16" t="n"/>
       <c r="F264" s="16" t="n"/>
       <c r="G264" s="30" t="n"/>
-      <c r="H264" s="252" t="n"/>
       <c r="I264" s="16" t="n"/>
-      <c r="J264" s="284" t="n"/>
+      <c r="J264" s="282" t="n"/>
       <c r="K264" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -37633,9 +37302,8 @@
       <c r="E265" s="16" t="n"/>
       <c r="F265" s="16" t="n"/>
       <c r="G265" s="30" t="n"/>
-      <c r="H265" s="252" t="n"/>
       <c r="I265" s="16" t="n"/>
-      <c r="J265" s="284" t="n"/>
+      <c r="J265" s="282" t="n"/>
       <c r="K265" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -37772,9 +37440,8 @@
       <c r="E266" s="16" t="n"/>
       <c r="F266" s="16" t="n"/>
       <c r="G266" s="30" t="n"/>
-      <c r="H266" s="252" t="n"/>
       <c r="I266" s="16" t="n"/>
-      <c r="J266" s="285" t="n"/>
+      <c r="J266" s="283" t="n"/>
       <c r="K266" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -38113,13 +37780,13 @@
       <c r="E269" s="16" t="n"/>
       <c r="F269" s="16" t="n"/>
       <c r="G269" s="30" t="n"/>
-      <c r="H269" s="281" t="inlineStr">
+      <c r="H269" s="279" t="inlineStr">
         <is>
           <t>LCOE</t>
         </is>
       </c>
       <c r="I269" s="16" t="n"/>
-      <c r="J269" s="283" t="inlineStr">
+      <c r="J269" s="281" t="inlineStr">
         <is>
           <t>Levelized Cost of Energy ($/MWh)</t>
         </is>
@@ -38294,9 +37961,8 @@
       <c r="E270" s="16" t="n"/>
       <c r="F270" s="16" t="n"/>
       <c r="G270" s="30" t="n"/>
-      <c r="H270" s="252" t="n"/>
       <c r="I270" s="16" t="n"/>
-      <c r="J270" s="284" t="n"/>
+      <c r="J270" s="282" t="n"/>
       <c r="K270" s="19" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Mid</t>
@@ -38467,9 +38133,8 @@
       <c r="E271" s="16" t="n"/>
       <c r="F271" s="16" t="n"/>
       <c r="G271" s="30" t="n"/>
-      <c r="H271" s="252" t="n"/>
       <c r="I271" s="16" t="n"/>
-      <c r="J271" s="284" t="n"/>
+      <c r="J271" s="282" t="n"/>
       <c r="K271" s="164" t="inlineStr">
         <is>
           <t>Res PV - Seattle - Constant</t>
@@ -38640,9 +38305,8 @@
       <c r="E272" s="16" t="n"/>
       <c r="F272" s="16" t="n"/>
       <c r="G272" s="30" t="n"/>
-      <c r="H272" s="252" t="n"/>
       <c r="I272" s="16" t="n"/>
-      <c r="J272" s="284" t="n"/>
+      <c r="J272" s="282" t="n"/>
       <c r="K272" s="160" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Low</t>
@@ -38813,9 +38477,8 @@
       <c r="E273" s="16" t="n"/>
       <c r="F273" s="16" t="n"/>
       <c r="G273" s="30" t="n"/>
-      <c r="H273" s="252" t="n"/>
       <c r="I273" s="16" t="n"/>
-      <c r="J273" s="284" t="n"/>
+      <c r="J273" s="282" t="n"/>
       <c r="K273" s="19" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Mid</t>
@@ -38986,9 +38649,8 @@
       <c r="E274" s="16" t="n"/>
       <c r="F274" s="16" t="n"/>
       <c r="G274" s="30" t="n"/>
-      <c r="H274" s="252" t="n"/>
       <c r="I274" s="16" t="n"/>
-      <c r="J274" s="284" t="n"/>
+      <c r="J274" s="282" t="n"/>
       <c r="K274" s="164" t="inlineStr">
         <is>
           <t>Res PV - Chicago - Constant</t>
@@ -39159,9 +38821,8 @@
       <c r="E275" s="16" t="n"/>
       <c r="F275" s="16" t="n"/>
       <c r="G275" s="30" t="n"/>
-      <c r="H275" s="252" t="n"/>
       <c r="I275" s="16" t="n"/>
-      <c r="J275" s="284" t="n"/>
+      <c r="J275" s="282" t="n"/>
       <c r="K275" s="160" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Low</t>
@@ -39332,9 +38993,8 @@
       <c r="E276" s="16" t="n"/>
       <c r="F276" s="16" t="n"/>
       <c r="G276" s="30" t="n"/>
-      <c r="H276" s="252" t="n"/>
       <c r="I276" s="16" t="n"/>
-      <c r="J276" s="284" t="n"/>
+      <c r="J276" s="282" t="n"/>
       <c r="K276" s="19" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Mid</t>
@@ -39505,9 +39165,8 @@
       <c r="E277" s="16" t="n"/>
       <c r="F277" s="16" t="n"/>
       <c r="G277" s="30" t="n"/>
-      <c r="H277" s="252" t="n"/>
       <c r="I277" s="16" t="n"/>
-      <c r="J277" s="284" t="n"/>
+      <c r="J277" s="282" t="n"/>
       <c r="K277" s="164" t="inlineStr">
         <is>
           <t>Res PV - Kansas City - Constant</t>
@@ -39678,9 +39337,8 @@
       <c r="E278" s="16" t="n"/>
       <c r="F278" s="16" t="n"/>
       <c r="G278" s="30" t="n"/>
-      <c r="H278" s="252" t="n"/>
       <c r="I278" s="16" t="n"/>
-      <c r="J278" s="284" t="n"/>
+      <c r="J278" s="282" t="n"/>
       <c r="K278" s="160" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Low</t>
@@ -39851,9 +39509,8 @@
       <c r="E279" s="16" t="n"/>
       <c r="F279" s="16" t="n"/>
       <c r="G279" s="30" t="n"/>
-      <c r="H279" s="252" t="n"/>
       <c r="I279" s="16" t="n"/>
-      <c r="J279" s="284" t="n"/>
+      <c r="J279" s="282" t="n"/>
       <c r="K279" s="19" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Mid</t>
@@ -40024,9 +39681,8 @@
       <c r="E280" s="16" t="n"/>
       <c r="F280" s="16" t="n"/>
       <c r="G280" s="30" t="n"/>
-      <c r="H280" s="252" t="n"/>
       <c r="I280" s="16" t="n"/>
-      <c r="J280" s="284" t="n"/>
+      <c r="J280" s="282" t="n"/>
       <c r="K280" s="164" t="inlineStr">
         <is>
           <t>Res PV - Los Angeles - Constant</t>
@@ -40197,9 +39853,8 @@
       <c r="E281" s="16" t="n"/>
       <c r="F281" s="16" t="n"/>
       <c r="G281" s="30" t="n"/>
-      <c r="H281" s="252" t="n"/>
       <c r="I281" s="16" t="n"/>
-      <c r="J281" s="284" t="n"/>
+      <c r="J281" s="282" t="n"/>
       <c r="K281" s="160" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Low</t>
@@ -40370,9 +40025,8 @@
       <c r="E282" s="16" t="n"/>
       <c r="F282" s="16" t="n"/>
       <c r="G282" s="30" t="n"/>
-      <c r="H282" s="252" t="n"/>
       <c r="I282" s="16" t="n"/>
-      <c r="J282" s="284" t="n"/>
+      <c r="J282" s="282" t="n"/>
       <c r="K282" s="19" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Mid</t>
@@ -40543,9 +40197,8 @@
       <c r="E283" s="16" t="n"/>
       <c r="F283" s="16" t="n"/>
       <c r="G283" s="30" t="n"/>
-      <c r="H283" s="252" t="n"/>
       <c r="I283" s="16" t="n"/>
-      <c r="J283" s="285" t="n"/>
+      <c r="J283" s="283" t="n"/>
       <c r="K283" s="164" t="inlineStr">
         <is>
           <t>Res PV - Daggett, CA - Constant</t>
@@ -41132,9 +40785,8 @@
       <c r="E288" s="16" t="n"/>
       <c r="F288" s="16" t="n"/>
       <c r="G288" s="30" t="n"/>
-      <c r="H288" s="252" t="n"/>
       <c r="I288" s="16" t="n"/>
-      <c r="J288" s="284" t="n"/>
+      <c r="J288" s="282" t="n"/>
       <c r="K288" s="19" t="inlineStr">
         <is>
           <t>10 year CRF - Mid</t>
@@ -41271,9 +40923,8 @@
       <c r="E289" s="16" t="n"/>
       <c r="F289" s="16" t="n"/>
       <c r="G289" s="30" t="n"/>
-      <c r="H289" s="252" t="n"/>
       <c r="I289" s="16" t="n"/>
-      <c r="J289" s="284" t="n"/>
+      <c r="J289" s="282" t="n"/>
       <c r="K289" s="19" t="inlineStr">
         <is>
           <t>10 year CRF - Constant</t>
@@ -41410,9 +41061,8 @@
       <c r="E290" s="16" t="n"/>
       <c r="F290" s="16" t="n"/>
       <c r="G290" s="30" t="n"/>
-      <c r="H290" s="252" t="n"/>
       <c r="I290" s="16" t="n"/>
-      <c r="J290" s="284" t="n"/>
+      <c r="J290" s="282" t="n"/>
       <c r="K290" s="19" t="inlineStr">
         <is>
           <t>Schedule</t>
@@ -41551,9 +41201,8 @@
       <c r="E291" s="16" t="n"/>
       <c r="F291" s="16" t="n"/>
       <c r="G291" s="30" t="n"/>
-      <c r="H291" s="252" t="n"/>
       <c r="I291" s="16" t="n"/>
-      <c r="J291" s="284" t="n"/>
+      <c r="J291" s="282" t="n"/>
       <c r="K291" s="19" t="inlineStr">
         <is>
           <t>PVD - Low</t>
@@ -41724,9 +41373,8 @@
       <c r="E292" s="16" t="n"/>
       <c r="F292" s="16" t="n"/>
       <c r="G292" s="30" t="n"/>
-      <c r="H292" s="252" t="n"/>
       <c r="I292" s="16" t="n"/>
-      <c r="J292" s="284" t="n"/>
+      <c r="J292" s="282" t="n"/>
       <c r="K292" s="19" t="inlineStr">
         <is>
           <t>PVD - Mid</t>
@@ -41897,9 +41545,8 @@
       <c r="E293" s="16" t="n"/>
       <c r="F293" s="16" t="n"/>
       <c r="G293" s="30" t="n"/>
-      <c r="H293" s="252" t="n"/>
       <c r="I293" s="16" t="n"/>
-      <c r="J293" s="284" t="n"/>
+      <c r="J293" s="282" t="n"/>
       <c r="K293" s="19" t="inlineStr">
         <is>
           <t>PVD - Constant</t>
@@ -42070,9 +41717,8 @@
       <c r="E294" s="16" t="n"/>
       <c r="F294" s="16" t="n"/>
       <c r="G294" s="30" t="n"/>
-      <c r="H294" s="252" t="n"/>
       <c r="I294" s="16" t="n"/>
-      <c r="J294" s="284" t="n"/>
+      <c r="J294" s="282" t="n"/>
       <c r="K294" s="19" t="inlineStr">
         <is>
           <t>PFF - Low</t>
@@ -42243,9 +41889,8 @@
       <c r="E295" s="16" t="n"/>
       <c r="F295" s="16" t="n"/>
       <c r="G295" s="30" t="n"/>
-      <c r="H295" s="252" t="n"/>
       <c r="I295" s="16" t="n"/>
-      <c r="J295" s="284" t="n"/>
+      <c r="J295" s="282" t="n"/>
       <c r="K295" s="19" t="inlineStr">
         <is>
           <t>PFF - Mid</t>
@@ -42416,9 +42061,8 @@
       <c r="E296" s="16" t="n"/>
       <c r="F296" s="16" t="n"/>
       <c r="G296" s="30" t="n"/>
-      <c r="H296" s="252" t="n"/>
       <c r="I296" s="16" t="n"/>
-      <c r="J296" s="284" t="n"/>
+      <c r="J296" s="282" t="n"/>
       <c r="K296" s="19" t="inlineStr">
         <is>
           <t>PFF - Constant</t>
@@ -42732,7 +42376,7 @@
       <c r="I298" s="213" t="n">
         <v>0.2</v>
       </c>
-      <c r="J298" s="286" t="inlineStr">
+      <c r="J298" s="284" t="inlineStr">
         <is>
           <t>Depreciation Factor</t>
         </is>
@@ -42909,7 +42553,6 @@
       <c r="I299" s="213" t="n">
         <v>0.32</v>
       </c>
-      <c r="J299" s="252" t="n"/>
       <c r="K299" s="217" t="n">
         <v>2</v>
       </c>
@@ -43082,7 +42725,6 @@
       <c r="I300" s="213" t="n">
         <v>0.192</v>
       </c>
-      <c r="J300" s="252" t="n"/>
       <c r="K300" s="217" t="n">
         <v>3</v>
       </c>
@@ -43255,7 +42897,6 @@
       <c r="I301" s="213" t="n">
         <v>0.1152</v>
       </c>
-      <c r="J301" s="252" t="n"/>
       <c r="K301" s="217" t="n">
         <v>4</v>
       </c>
@@ -43428,7 +43069,6 @@
       <c r="I302" s="213" t="n">
         <v>0.1152</v>
       </c>
-      <c r="J302" s="252" t="n"/>
       <c r="K302" s="217" t="n">
         <v>5</v>
       </c>
@@ -43601,7 +43241,6 @@
       <c r="I303" s="213" t="n">
         <v>0.0576</v>
       </c>
-      <c r="J303" s="252" t="n"/>
       <c r="K303" s="217" t="n">
         <v>6</v>
       </c>
@@ -43772,7 +43411,6 @@
       <c r="G304" s="30" t="n"/>
       <c r="H304" s="212" t="n"/>
       <c r="I304" s="213" t="n"/>
-      <c r="J304" s="252" t="n"/>
       <c r="K304" s="215" t="inlineStr">
         <is>
           <t>Year (Mid)</t>
@@ -43911,7 +43549,6 @@
       <c r="G305" s="30" t="n"/>
       <c r="H305" s="212" t="n"/>
       <c r="I305" s="16" t="n"/>
-      <c r="J305" s="252" t="n"/>
       <c r="K305" s="217" t="n">
         <v>1</v>
       </c>
@@ -44082,7 +43719,6 @@
       <c r="G306" s="30" t="n"/>
       <c r="H306" s="212" t="n"/>
       <c r="I306" s="16" t="n"/>
-      <c r="J306" s="252" t="n"/>
       <c r="K306" s="217" t="n">
         <v>2</v>
       </c>
@@ -44253,7 +43889,6 @@
       <c r="G307" s="30" t="n"/>
       <c r="H307" s="212" t="n"/>
       <c r="I307" s="16" t="n"/>
-      <c r="J307" s="252" t="n"/>
       <c r="K307" s="217" t="n">
         <v>3</v>
       </c>
@@ -44424,7 +44059,6 @@
       <c r="G308" s="30" t="n"/>
       <c r="H308" s="212" t="n"/>
       <c r="I308" s="16" t="n"/>
-      <c r="J308" s="252" t="n"/>
       <c r="K308" s="217" t="n">
         <v>4</v>
       </c>
@@ -44595,7 +44229,6 @@
       <c r="G309" s="30" t="n"/>
       <c r="H309" s="212" t="n"/>
       <c r="I309" s="16" t="n"/>
-      <c r="J309" s="252" t="n"/>
       <c r="K309" s="217" t="n">
         <v>5</v>
       </c>
@@ -44766,7 +44399,6 @@
       <c r="G310" s="30" t="n"/>
       <c r="H310" s="212" t="n"/>
       <c r="I310" s="16" t="n"/>
-      <c r="J310" s="252" t="n"/>
       <c r="K310" s="217" t="n">
         <v>6</v>
       </c>
@@ -44937,7 +44569,6 @@
       <c r="G311" s="30" t="n"/>
       <c r="H311" s="212" t="n"/>
       <c r="I311" s="16" t="n"/>
-      <c r="J311" s="252" t="n"/>
       <c r="K311" s="217" t="inlineStr">
         <is>
           <t>Year (Constant)</t>
@@ -45076,7 +44707,6 @@
       <c r="G312" s="30" t="n"/>
       <c r="H312" s="212" t="n"/>
       <c r="I312" s="16" t="n"/>
-      <c r="J312" s="252" t="n"/>
       <c r="K312" s="217" t="n">
         <v>1</v>
       </c>
@@ -45247,7 +44877,6 @@
       <c r="G313" s="30" t="n"/>
       <c r="H313" s="212" t="n"/>
       <c r="I313" s="16" t="n"/>
-      <c r="J313" s="252" t="n"/>
       <c r="K313" s="217" t="n">
         <v>2</v>
       </c>
@@ -45418,7 +45047,6 @@
       <c r="G314" s="30" t="n"/>
       <c r="H314" s="212" t="n"/>
       <c r="I314" s="16" t="n"/>
-      <c r="J314" s="252" t="n"/>
       <c r="K314" s="217" t="n">
         <v>3</v>
       </c>
@@ -45589,7 +45217,6 @@
       <c r="G315" s="30" t="n"/>
       <c r="H315" s="212" t="n"/>
       <c r="I315" s="16" t="n"/>
-      <c r="J315" s="252" t="n"/>
       <c r="K315" s="217" t="n">
         <v>4</v>
       </c>
@@ -45760,7 +45387,6 @@
       <c r="G316" s="30" t="n"/>
       <c r="H316" s="212" t="n"/>
       <c r="I316" s="16" t="n"/>
-      <c r="J316" s="252" t="n"/>
       <c r="K316" s="217" t="n">
         <v>5</v>
       </c>
@@ -45931,7 +45557,7 @@
       <c r="G317" s="152" t="n"/>
       <c r="H317" s="153" t="n"/>
       <c r="I317" s="153" t="n"/>
-      <c r="J317" s="287" t="n"/>
+      <c r="J317" s="285" t="n"/>
       <c r="K317" s="217" t="n">
         <v>6</v>
       </c>
@@ -46587,18 +46213,6 @@
           <t>Graphics</t>
         </is>
       </c>
-      <c r="I324" s="252" t="n"/>
-      <c r="J324" s="252" t="n"/>
-      <c r="K324" s="252" t="n"/>
-      <c r="L324" s="252" t="n"/>
-      <c r="M324" s="252" t="n"/>
-      <c r="N324" s="252" t="n"/>
-      <c r="O324" s="252" t="n"/>
-      <c r="P324" s="252" t="n"/>
-      <c r="Q324" s="252" t="n"/>
-      <c r="R324" s="252" t="n"/>
-      <c r="S324" s="252" t="n"/>
-      <c r="T324" s="252" t="n"/>
       <c r="U324" s="224" t="n"/>
       <c r="V324" s="224" t="n"/>
       <c r="W324" s="224" t="n"/>
@@ -60676,26 +60290,6 @@
           <t>Data Sources for Default Inputs</t>
         </is>
       </c>
-      <c r="H534" s="252" t="n"/>
-      <c r="I534" s="252" t="n"/>
-      <c r="J534" s="252" t="n"/>
-      <c r="K534" s="252" t="n"/>
-      <c r="L534" s="252" t="n"/>
-      <c r="M534" s="252" t="n"/>
-      <c r="N534" s="252" t="n"/>
-      <c r="O534" s="252" t="n"/>
-      <c r="P534" s="252" t="n"/>
-      <c r="Q534" s="252" t="n"/>
-      <c r="R534" s="252" t="n"/>
-      <c r="S534" s="252" t="n"/>
-      <c r="T534" s="252" t="n"/>
-      <c r="U534" s="252" t="n"/>
-      <c r="V534" s="252" t="n"/>
-      <c r="W534" s="252" t="n"/>
-      <c r="X534" s="252" t="n"/>
-      <c r="Y534" s="252" t="n"/>
-      <c r="Z534" s="252" t="n"/>
-      <c r="AA534" s="252" t="n"/>
       <c r="AB534" s="16" t="n"/>
       <c r="AC534" s="16" t="n"/>
       <c r="AD534" s="16" t="n"/>
@@ -60877,30 +60471,30 @@
       <c r="E537" s="16" t="n"/>
       <c r="F537" s="16" t="n"/>
       <c r="G537" s="16" t="n"/>
-      <c r="H537" s="288" t="inlineStr">
+      <c r="H537" s="286" t="inlineStr">
         <is>
           <t>Current Costs:</t>
         </is>
       </c>
-      <c r="I537" s="289" t="n"/>
-      <c r="J537" s="289" t="n"/>
-      <c r="K537" s="289" t="n"/>
-      <c r="L537" s="290" t="n"/>
-      <c r="M537" s="291" t="n"/>
-      <c r="N537" s="289" t="n"/>
-      <c r="O537" s="289" t="n"/>
-      <c r="P537" s="289" t="n"/>
-      <c r="Q537" s="289" t="n"/>
-      <c r="R537" s="289" t="n"/>
-      <c r="S537" s="289" t="n"/>
-      <c r="T537" s="289" t="n"/>
-      <c r="U537" s="289" t="n"/>
-      <c r="V537" s="289" t="n"/>
-      <c r="W537" s="289" t="n"/>
-      <c r="X537" s="289" t="n"/>
-      <c r="Y537" s="289" t="n"/>
-      <c r="Z537" s="289" t="n"/>
-      <c r="AA537" s="290" t="n"/>
+      <c r="I537" s="287" t="n"/>
+      <c r="J537" s="287" t="n"/>
+      <c r="K537" s="287" t="n"/>
+      <c r="L537" s="288" t="n"/>
+      <c r="M537" s="289" t="n"/>
+      <c r="N537" s="287" t="n"/>
+      <c r="O537" s="287" t="n"/>
+      <c r="P537" s="287" t="n"/>
+      <c r="Q537" s="287" t="n"/>
+      <c r="R537" s="287" t="n"/>
+      <c r="S537" s="287" t="n"/>
+      <c r="T537" s="287" t="n"/>
+      <c r="U537" s="287" t="n"/>
+      <c r="V537" s="287" t="n"/>
+      <c r="W537" s="287" t="n"/>
+      <c r="X537" s="287" t="n"/>
+      <c r="Y537" s="287" t="n"/>
+      <c r="Z537" s="287" t="n"/>
+      <c r="AA537" s="288" t="n"/>
       <c r="AB537" s="16" t="n"/>
       <c r="AC537" s="16" t="n"/>
       <c r="AD537" s="16" t="n"/>
@@ -60948,34 +60542,34 @@
       <c r="E538" s="16" t="n"/>
       <c r="F538" s="16" t="n"/>
       <c r="G538" s="16" t="n"/>
-      <c r="H538" s="292" t="inlineStr">
+      <c r="H538" s="290" t="inlineStr">
         <is>
           <t>Available Capacity (GW)</t>
         </is>
       </c>
-      <c r="I538" s="293" t="n"/>
-      <c r="J538" s="293" t="n"/>
-      <c r="K538" s="293" t="n"/>
-      <c r="L538" s="294" t="n"/>
-      <c r="M538" s="295" t="inlineStr">
+      <c r="I538" s="291" t="n"/>
+      <c r="J538" s="291" t="n"/>
+      <c r="K538" s="291" t="n"/>
+      <c r="L538" s="292" t="n"/>
+      <c r="M538" s="293" t="inlineStr">
         <is>
           <t>Pieter Gagnon, Robert Margolis, Jennifer Melius, Caleb Phillips, Ryan Elmore. (2016). Rooftop Solar Photovoltaic Technical Potential in the United States: A Detailed Assessment. NREL TP-6A20-65298</t>
         </is>
       </c>
-      <c r="N538" s="293" t="n"/>
-      <c r="O538" s="293" t="n"/>
-      <c r="P538" s="293" t="n"/>
-      <c r="Q538" s="293" t="n"/>
-      <c r="R538" s="293" t="n"/>
-      <c r="S538" s="293" t="n"/>
-      <c r="T538" s="293" t="n"/>
-      <c r="U538" s="293" t="n"/>
-      <c r="V538" s="293" t="n"/>
-      <c r="W538" s="293" t="n"/>
-      <c r="X538" s="293" t="n"/>
-      <c r="Y538" s="293" t="n"/>
-      <c r="Z538" s="293" t="n"/>
-      <c r="AA538" s="296" t="n"/>
+      <c r="N538" s="291" t="n"/>
+      <c r="O538" s="291" t="n"/>
+      <c r="P538" s="291" t="n"/>
+      <c r="Q538" s="291" t="n"/>
+      <c r="R538" s="291" t="n"/>
+      <c r="S538" s="291" t="n"/>
+      <c r="T538" s="291" t="n"/>
+      <c r="U538" s="291" t="n"/>
+      <c r="V538" s="291" t="n"/>
+      <c r="W538" s="291" t="n"/>
+      <c r="X538" s="291" t="n"/>
+      <c r="Y538" s="291" t="n"/>
+      <c r="Z538" s="291" t="n"/>
+      <c r="AA538" s="294" t="n"/>
       <c r="AB538" s="16" t="n"/>
       <c r="AC538" s="16" t="n"/>
       <c r="AD538" s="16" t="n"/>
@@ -61023,34 +60617,34 @@
       <c r="E539" s="16" t="n"/>
       <c r="F539" s="16" t="n"/>
       <c r="G539" s="16" t="n"/>
-      <c r="H539" s="292" t="inlineStr">
+      <c r="H539" s="290" t="inlineStr">
         <is>
           <t>Net Capacity Factor (%)</t>
         </is>
       </c>
-      <c r="I539" s="293" t="n"/>
-      <c r="J539" s="293" t="n"/>
-      <c r="K539" s="293" t="n"/>
-      <c r="L539" s="294" t="n"/>
-      <c r="M539" s="295" t="inlineStr">
+      <c r="I539" s="291" t="n"/>
+      <c r="J539" s="291" t="n"/>
+      <c r="K539" s="291" t="n"/>
+      <c r="L539" s="292" t="n"/>
+      <c r="M539" s="293" t="inlineStr">
         <is>
           <t>National Renewable Energy Laboratory. PVWATTS v5. Representative of national range of capacity factors.</t>
         </is>
       </c>
-      <c r="N539" s="293" t="n"/>
-      <c r="O539" s="293" t="n"/>
-      <c r="P539" s="293" t="n"/>
-      <c r="Q539" s="293" t="n"/>
-      <c r="R539" s="293" t="n"/>
-      <c r="S539" s="293" t="n"/>
-      <c r="T539" s="293" t="n"/>
-      <c r="U539" s="293" t="n"/>
-      <c r="V539" s="293" t="n"/>
-      <c r="W539" s="293" t="n"/>
-      <c r="X539" s="293" t="n"/>
-      <c r="Y539" s="293" t="n"/>
-      <c r="Z539" s="293" t="n"/>
-      <c r="AA539" s="296" t="n"/>
+      <c r="N539" s="291" t="n"/>
+      <c r="O539" s="291" t="n"/>
+      <c r="P539" s="291" t="n"/>
+      <c r="Q539" s="291" t="n"/>
+      <c r="R539" s="291" t="n"/>
+      <c r="S539" s="291" t="n"/>
+      <c r="T539" s="291" t="n"/>
+      <c r="U539" s="291" t="n"/>
+      <c r="V539" s="291" t="n"/>
+      <c r="W539" s="291" t="n"/>
+      <c r="X539" s="291" t="n"/>
+      <c r="Y539" s="291" t="n"/>
+      <c r="Z539" s="291" t="n"/>
+      <c r="AA539" s="294" t="n"/>
       <c r="AB539" s="16" t="n"/>
       <c r="AC539" s="16" t="n"/>
       <c r="AD539" s="16" t="n"/>
@@ -61098,34 +60692,34 @@
       <c r="E540" s="16" t="n"/>
       <c r="F540" s="16" t="n"/>
       <c r="G540" s="16" t="n"/>
-      <c r="H540" s="292" t="inlineStr">
+      <c r="H540" s="290" t="inlineStr">
         <is>
           <t>Overnight Capital Cost ($/kW)</t>
         </is>
       </c>
-      <c r="I540" s="293" t="n"/>
-      <c r="J540" s="293" t="n"/>
-      <c r="K540" s="293" t="n"/>
-      <c r="L540" s="294" t="n"/>
-      <c r="M540" s="297" t="inlineStr">
+      <c r="I540" s="291" t="n"/>
+      <c r="J540" s="291" t="n"/>
+      <c r="K540" s="291" t="n"/>
+      <c r="L540" s="292" t="n"/>
+      <c r="M540" s="295" t="inlineStr">
         <is>
           <t>Fu, R., D. Feldman, and R. Margolis. 2018. U.S. Photovoltaic (PV) Prices and Cost Breakdowns: Q1 2018 Benchmarks for Residential, Commercial, and Utility-Scale Systems. Golden, CO: National Renewable Energy Laboratory</t>
         </is>
       </c>
-      <c r="N540" s="293" t="n"/>
-      <c r="O540" s="293" t="n"/>
-      <c r="P540" s="293" t="n"/>
-      <c r="Q540" s="293" t="n"/>
-      <c r="R540" s="293" t="n"/>
-      <c r="S540" s="293" t="n"/>
-      <c r="T540" s="293" t="n"/>
-      <c r="U540" s="293" t="n"/>
-      <c r="V540" s="293" t="n"/>
-      <c r="W540" s="293" t="n"/>
-      <c r="X540" s="293" t="n"/>
-      <c r="Y540" s="293" t="n"/>
-      <c r="Z540" s="293" t="n"/>
-      <c r="AA540" s="294" t="n"/>
+      <c r="N540" s="291" t="n"/>
+      <c r="O540" s="291" t="n"/>
+      <c r="P540" s="291" t="n"/>
+      <c r="Q540" s="291" t="n"/>
+      <c r="R540" s="291" t="n"/>
+      <c r="S540" s="291" t="n"/>
+      <c r="T540" s="291" t="n"/>
+      <c r="U540" s="291" t="n"/>
+      <c r="V540" s="291" t="n"/>
+      <c r="W540" s="291" t="n"/>
+      <c r="X540" s="291" t="n"/>
+      <c r="Y540" s="291" t="n"/>
+      <c r="Z540" s="291" t="n"/>
+      <c r="AA540" s="292" t="n"/>
       <c r="AB540" s="16" t="n"/>
       <c r="AC540" s="16" t="n"/>
       <c r="AD540" s="16" t="n"/>
@@ -61173,34 +60767,34 @@
       <c r="E541" s="16" t="n"/>
       <c r="F541" s="16" t="n"/>
       <c r="G541" s="16" t="n"/>
-      <c r="H541" s="292" t="inlineStr">
+      <c r="H541" s="290" t="inlineStr">
         <is>
           <t>Fixed Operating Expenses ($/kW-yr)</t>
         </is>
       </c>
-      <c r="I541" s="293" t="n"/>
-      <c r="J541" s="293" t="n"/>
-      <c r="K541" s="293" t="n"/>
-      <c r="L541" s="294" t="n"/>
-      <c r="M541" s="297" t="inlineStr">
+      <c r="I541" s="291" t="n"/>
+      <c r="J541" s="291" t="n"/>
+      <c r="K541" s="291" t="n"/>
+      <c r="L541" s="292" t="n"/>
+      <c r="M541" s="295" t="inlineStr">
         <is>
           <t>Fu, R., D. Feldman, and R. Margolis. 2018. U.S. Photovoltaic (PV) Prices and Cost Breakdowns: Q1 2018 Benchmarks for Residential, Commercial, and Utility-Scale Systems. Golden, CO: National Renewable Energy Laboratory</t>
         </is>
       </c>
-      <c r="N541" s="293" t="n"/>
-      <c r="O541" s="293" t="n"/>
-      <c r="P541" s="293" t="n"/>
-      <c r="Q541" s="293" t="n"/>
-      <c r="R541" s="293" t="n"/>
-      <c r="S541" s="293" t="n"/>
-      <c r="T541" s="293" t="n"/>
-      <c r="U541" s="293" t="n"/>
-      <c r="V541" s="293" t="n"/>
-      <c r="W541" s="293" t="n"/>
-      <c r="X541" s="293" t="n"/>
-      <c r="Y541" s="293" t="n"/>
-      <c r="Z541" s="293" t="n"/>
-      <c r="AA541" s="294" t="n"/>
+      <c r="N541" s="291" t="n"/>
+      <c r="O541" s="291" t="n"/>
+      <c r="P541" s="291" t="n"/>
+      <c r="Q541" s="291" t="n"/>
+      <c r="R541" s="291" t="n"/>
+      <c r="S541" s="291" t="n"/>
+      <c r="T541" s="291" t="n"/>
+      <c r="U541" s="291" t="n"/>
+      <c r="V541" s="291" t="n"/>
+      <c r="W541" s="291" t="n"/>
+      <c r="X541" s="291" t="n"/>
+      <c r="Y541" s="291" t="n"/>
+      <c r="Z541" s="291" t="n"/>
+      <c r="AA541" s="292" t="n"/>
       <c r="AB541" s="16" t="n"/>
       <c r="AC541" s="16" t="n"/>
       <c r="AD541" s="16" t="n"/>
@@ -61248,34 +60842,34 @@
       <c r="E542" s="16" t="n"/>
       <c r="F542" s="16" t="n"/>
       <c r="G542" s="16" t="n"/>
-      <c r="H542" s="292" t="inlineStr">
+      <c r="H542" s="290" t="inlineStr">
         <is>
           <t>Variable Operating Expenses ($/MWh)</t>
         </is>
       </c>
-      <c r="I542" s="293" t="n"/>
-      <c r="J542" s="293" t="n"/>
-      <c r="K542" s="293" t="n"/>
-      <c r="L542" s="294" t="n"/>
-      <c r="M542" s="298" t="inlineStr">
+      <c r="I542" s="291" t="n"/>
+      <c r="J542" s="291" t="n"/>
+      <c r="K542" s="291" t="n"/>
+      <c r="L542" s="292" t="n"/>
+      <c r="M542" s="296" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="N542" s="293" t="n"/>
-      <c r="O542" s="293" t="n"/>
-      <c r="P542" s="293" t="n"/>
-      <c r="Q542" s="293" t="n"/>
-      <c r="R542" s="293" t="n"/>
-      <c r="S542" s="293" t="n"/>
-      <c r="T542" s="293" t="n"/>
-      <c r="U542" s="293" t="n"/>
-      <c r="V542" s="293" t="n"/>
-      <c r="W542" s="293" t="n"/>
-      <c r="X542" s="293" t="n"/>
-      <c r="Y542" s="293" t="n"/>
-      <c r="Z542" s="293" t="n"/>
-      <c r="AA542" s="294" t="n"/>
+      <c r="N542" s="291" t="n"/>
+      <c r="O542" s="291" t="n"/>
+      <c r="P542" s="291" t="n"/>
+      <c r="Q542" s="291" t="n"/>
+      <c r="R542" s="291" t="n"/>
+      <c r="S542" s="291" t="n"/>
+      <c r="T542" s="291" t="n"/>
+      <c r="U542" s="291" t="n"/>
+      <c r="V542" s="291" t="n"/>
+      <c r="W542" s="291" t="n"/>
+      <c r="X542" s="291" t="n"/>
+      <c r="Y542" s="291" t="n"/>
+      <c r="Z542" s="291" t="n"/>
+      <c r="AA542" s="292" t="n"/>
       <c r="AB542" s="16" t="n"/>
       <c r="AC542" s="16" t="n"/>
       <c r="AD542" s="16" t="n"/>
@@ -61323,34 +60917,34 @@
       <c r="E543" s="16" t="n"/>
       <c r="F543" s="16" t="n"/>
       <c r="G543" s="16" t="n"/>
-      <c r="H543" s="292" t="inlineStr">
+      <c r="H543" s="290" t="inlineStr">
         <is>
           <t>Grid Feature Cost ($/kW)</t>
         </is>
       </c>
-      <c r="I543" s="293" t="n"/>
-      <c r="J543" s="293" t="n"/>
-      <c r="K543" s="293" t="n"/>
-      <c r="L543" s="294" t="n"/>
-      <c r="M543" s="298" t="inlineStr">
+      <c r="I543" s="291" t="n"/>
+      <c r="J543" s="291" t="n"/>
+      <c r="K543" s="291" t="n"/>
+      <c r="L543" s="292" t="n"/>
+      <c r="M543" s="296" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="N543" s="293" t="n"/>
-      <c r="O543" s="293" t="n"/>
-      <c r="P543" s="293" t="n"/>
-      <c r="Q543" s="293" t="n"/>
-      <c r="R543" s="293" t="n"/>
-      <c r="S543" s="293" t="n"/>
-      <c r="T543" s="293" t="n"/>
-      <c r="U543" s="293" t="n"/>
-      <c r="V543" s="293" t="n"/>
-      <c r="W543" s="293" t="n"/>
-      <c r="X543" s="293" t="n"/>
-      <c r="Y543" s="293" t="n"/>
-      <c r="Z543" s="293" t="n"/>
-      <c r="AA543" s="294" t="n"/>
+      <c r="N543" s="291" t="n"/>
+      <c r="O543" s="291" t="n"/>
+      <c r="P543" s="291" t="n"/>
+      <c r="Q543" s="291" t="n"/>
+      <c r="R543" s="291" t="n"/>
+      <c r="S543" s="291" t="n"/>
+      <c r="T543" s="291" t="n"/>
+      <c r="U543" s="291" t="n"/>
+      <c r="V543" s="291" t="n"/>
+      <c r="W543" s="291" t="n"/>
+      <c r="X543" s="291" t="n"/>
+      <c r="Y543" s="291" t="n"/>
+      <c r="Z543" s="291" t="n"/>
+      <c r="AA543" s="292" t="n"/>
       <c r="AB543" s="16" t="n"/>
       <c r="AC543" s="16" t="n"/>
       <c r="AD543" s="16" t="n"/>
@@ -61398,34 +60992,34 @@
       <c r="E544" s="16" t="n"/>
       <c r="F544" s="16" t="n"/>
       <c r="G544" s="16" t="n"/>
-      <c r="H544" s="299" t="inlineStr">
+      <c r="H544" s="297" t="inlineStr">
         <is>
           <t>Spur Line Cost ($/kW)</t>
         </is>
       </c>
-      <c r="I544" s="300" t="n"/>
-      <c r="J544" s="300" t="n"/>
-      <c r="K544" s="300" t="n"/>
-      <c r="L544" s="301" t="n"/>
-      <c r="M544" s="302" t="inlineStr">
+      <c r="I544" s="298" t="n"/>
+      <c r="J544" s="298" t="n"/>
+      <c r="K544" s="298" t="n"/>
+      <c r="L544" s="299" t="n"/>
+      <c r="M544" s="300" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="N544" s="300" t="n"/>
-      <c r="O544" s="300" t="n"/>
-      <c r="P544" s="300" t="n"/>
-      <c r="Q544" s="300" t="n"/>
-      <c r="R544" s="300" t="n"/>
-      <c r="S544" s="300" t="n"/>
-      <c r="T544" s="300" t="n"/>
-      <c r="U544" s="300" t="n"/>
-      <c r="V544" s="300" t="n"/>
-      <c r="W544" s="300" t="n"/>
-      <c r="X544" s="300" t="n"/>
-      <c r="Y544" s="300" t="n"/>
-      <c r="Z544" s="300" t="n"/>
-      <c r="AA544" s="303" t="n"/>
+      <c r="N544" s="298" t="n"/>
+      <c r="O544" s="298" t="n"/>
+      <c r="P544" s="298" t="n"/>
+      <c r="Q544" s="298" t="n"/>
+      <c r="R544" s="298" t="n"/>
+      <c r="S544" s="298" t="n"/>
+      <c r="T544" s="298" t="n"/>
+      <c r="U544" s="298" t="n"/>
+      <c r="V544" s="298" t="n"/>
+      <c r="W544" s="298" t="n"/>
+      <c r="X544" s="298" t="n"/>
+      <c r="Y544" s="298" t="n"/>
+      <c r="Z544" s="298" t="n"/>
+      <c r="AA544" s="301" t="n"/>
       <c r="AB544" s="16" t="n"/>
       <c r="AC544" s="16" t="n"/>
       <c r="AD544" s="16" t="n"/>
@@ -61473,11 +61067,7 @@
       <c r="E545" s="16" t="n"/>
       <c r="F545" s="16" t="n"/>
       <c r="G545" s="16" t="n"/>
-      <c r="H545" s="304" t="n"/>
-      <c r="I545" s="252" t="n"/>
-      <c r="J545" s="252" t="n"/>
-      <c r="K545" s="252" t="n"/>
-      <c r="L545" s="252" t="n"/>
+      <c r="H545" s="246" t="n"/>
       <c r="M545" s="247" t="n"/>
       <c r="N545" s="247" t="n"/>
       <c r="O545" s="247" t="n"/>
@@ -61540,30 +61130,30 @@
       <c r="E546" s="16" t="n"/>
       <c r="F546" s="16" t="n"/>
       <c r="G546" s="16" t="n"/>
-      <c r="H546" s="288" t="inlineStr">
+      <c r="H546" s="286" t="inlineStr">
         <is>
           <t>Future Projections Costs:</t>
         </is>
       </c>
-      <c r="I546" s="289" t="n"/>
-      <c r="J546" s="289" t="n"/>
-      <c r="K546" s="289" t="n"/>
-      <c r="L546" s="290" t="n"/>
-      <c r="M546" s="305" t="n"/>
-      <c r="N546" s="289" t="n"/>
-      <c r="O546" s="289" t="n"/>
-      <c r="P546" s="289" t="n"/>
-      <c r="Q546" s="289" t="n"/>
-      <c r="R546" s="289" t="n"/>
-      <c r="S546" s="289" t="n"/>
-      <c r="T546" s="289" t="n"/>
-      <c r="U546" s="289" t="n"/>
-      <c r="V546" s="289" t="n"/>
-      <c r="W546" s="289" t="n"/>
-      <c r="X546" s="289" t="n"/>
-      <c r="Y546" s="289" t="n"/>
-      <c r="Z546" s="289" t="n"/>
-      <c r="AA546" s="306" t="n"/>
+      <c r="I546" s="287" t="n"/>
+      <c r="J546" s="287" t="n"/>
+      <c r="K546" s="287" t="n"/>
+      <c r="L546" s="288" t="n"/>
+      <c r="M546" s="302" t="n"/>
+      <c r="N546" s="287" t="n"/>
+      <c r="O546" s="287" t="n"/>
+      <c r="P546" s="287" t="n"/>
+      <c r="Q546" s="287" t="n"/>
+      <c r="R546" s="287" t="n"/>
+      <c r="S546" s="287" t="n"/>
+      <c r="T546" s="287" t="n"/>
+      <c r="U546" s="287" t="n"/>
+      <c r="V546" s="287" t="n"/>
+      <c r="W546" s="287" t="n"/>
+      <c r="X546" s="287" t="n"/>
+      <c r="Y546" s="287" t="n"/>
+      <c r="Z546" s="287" t="n"/>
+      <c r="AA546" s="303" t="n"/>
       <c r="AB546" s="16" t="n"/>
       <c r="AC546" s="16" t="n"/>
       <c r="AD546" s="16" t="n"/>
@@ -61611,34 +61201,34 @@
       <c r="E547" s="16" t="n"/>
       <c r="F547" s="16" t="n"/>
       <c r="G547" s="16" t="n"/>
-      <c r="H547" s="292" t="inlineStr">
+      <c r="H547" s="290" t="inlineStr">
         <is>
           <t>Net Capacity Factor (%)</t>
         </is>
       </c>
-      <c r="I547" s="293" t="n"/>
-      <c r="J547" s="293" t="n"/>
-      <c r="K547" s="293" t="n"/>
-      <c r="L547" s="294" t="n"/>
-      <c r="M547" s="295" t="inlineStr">
+      <c r="I547" s="291" t="n"/>
+      <c r="J547" s="291" t="n"/>
+      <c r="K547" s="291" t="n"/>
+      <c r="L547" s="292" t="n"/>
+      <c r="M547" s="293" t="inlineStr">
         <is>
           <t>Jones-Albertus, R et al (2015). Technology Advances Needed for Photovoltaics to Achieve Widespread Grid Price Parity.</t>
         </is>
       </c>
-      <c r="N547" s="293" t="n"/>
-      <c r="O547" s="293" t="n"/>
-      <c r="P547" s="293" t="n"/>
-      <c r="Q547" s="293" t="n"/>
-      <c r="R547" s="293" t="n"/>
-      <c r="S547" s="293" t="n"/>
-      <c r="T547" s="293" t="n"/>
-      <c r="U547" s="293" t="n"/>
-      <c r="V547" s="293" t="n"/>
-      <c r="W547" s="293" t="n"/>
-      <c r="X547" s="293" t="n"/>
-      <c r="Y547" s="293" t="n"/>
-      <c r="Z547" s="293" t="n"/>
-      <c r="AA547" s="296" t="n"/>
+      <c r="N547" s="291" t="n"/>
+      <c r="O547" s="291" t="n"/>
+      <c r="P547" s="291" t="n"/>
+      <c r="Q547" s="291" t="n"/>
+      <c r="R547" s="291" t="n"/>
+      <c r="S547" s="291" t="n"/>
+      <c r="T547" s="291" t="n"/>
+      <c r="U547" s="291" t="n"/>
+      <c r="V547" s="291" t="n"/>
+      <c r="W547" s="291" t="n"/>
+      <c r="X547" s="291" t="n"/>
+      <c r="Y547" s="291" t="n"/>
+      <c r="Z547" s="291" t="n"/>
+      <c r="AA547" s="294" t="n"/>
       <c r="AB547" s="16" t="n"/>
       <c r="AC547" s="16" t="n"/>
       <c r="AD547" s="16" t="n"/>
@@ -61686,34 +61276,34 @@
       <c r="E548" s="16" t="n"/>
       <c r="F548" s="16" t="n"/>
       <c r="G548" s="16" t="n"/>
-      <c r="H548" s="292" t="inlineStr">
+      <c r="H548" s="290" t="inlineStr">
         <is>
           <t>Overnight Capital Cost ($/kW)</t>
         </is>
       </c>
-      <c r="I548" s="293" t="n"/>
-      <c r="J548" s="293" t="n"/>
-      <c r="K548" s="293" t="n"/>
-      <c r="L548" s="294" t="n"/>
-      <c r="M548" s="295" t="inlineStr">
+      <c r="I548" s="291" t="n"/>
+      <c r="J548" s="291" t="n"/>
+      <c r="K548" s="291" t="n"/>
+      <c r="L548" s="292" t="n"/>
+      <c r="M548" s="293" t="inlineStr">
         <is>
           <t>Literature review of Residential PV capital cost projections.  See accompanying ATB presentation for more information.</t>
         </is>
       </c>
-      <c r="N548" s="293" t="n"/>
-      <c r="O548" s="293" t="n"/>
-      <c r="P548" s="293" t="n"/>
-      <c r="Q548" s="293" t="n"/>
-      <c r="R548" s="293" t="n"/>
-      <c r="S548" s="293" t="n"/>
-      <c r="T548" s="293" t="n"/>
-      <c r="U548" s="293" t="n"/>
-      <c r="V548" s="293" t="n"/>
-      <c r="W548" s="293" t="n"/>
-      <c r="X548" s="293" t="n"/>
-      <c r="Y548" s="293" t="n"/>
-      <c r="Z548" s="293" t="n"/>
-      <c r="AA548" s="296" t="n"/>
+      <c r="N548" s="291" t="n"/>
+      <c r="O548" s="291" t="n"/>
+      <c r="P548" s="291" t="n"/>
+      <c r="Q548" s="291" t="n"/>
+      <c r="R548" s="291" t="n"/>
+      <c r="S548" s="291" t="n"/>
+      <c r="T548" s="291" t="n"/>
+      <c r="U548" s="291" t="n"/>
+      <c r="V548" s="291" t="n"/>
+      <c r="W548" s="291" t="n"/>
+      <c r="X548" s="291" t="n"/>
+      <c r="Y548" s="291" t="n"/>
+      <c r="Z548" s="291" t="n"/>
+      <c r="AA548" s="294" t="n"/>
       <c r="AB548" s="16" t="n"/>
       <c r="AC548" s="16" t="n"/>
       <c r="AD548" s="16" t="n"/>
@@ -61761,34 +61351,34 @@
       <c r="E549" s="16" t="n"/>
       <c r="F549" s="16" t="n"/>
       <c r="G549" s="16" t="n"/>
-      <c r="H549" s="292" t="inlineStr">
+      <c r="H549" s="290" t="inlineStr">
         <is>
           <t>Fixed Operating Expenses ($/kW-yr)</t>
         </is>
       </c>
-      <c r="I549" s="293" t="n"/>
-      <c r="J549" s="293" t="n"/>
-      <c r="K549" s="293" t="n"/>
-      <c r="L549" s="294" t="n"/>
-      <c r="M549" s="297" t="inlineStr">
+      <c r="I549" s="291" t="n"/>
+      <c r="J549" s="291" t="n"/>
+      <c r="K549" s="291" t="n"/>
+      <c r="L549" s="292" t="n"/>
+      <c r="M549" s="295" t="inlineStr">
         <is>
           <t>The ratio between O&amp;M costs to CAPEX from: Fu, R., D. Feldman, and R. Margolis. 2018. U.S. Photovoltaic (PV) Prices and Cost Breakdowns: Q1 2018 Benchmarks for Residential, Commercial, and Utility-Scale Systems. Golden, CO: National Renewable Energy Laboratory.  See accompanying ATB presentation for more information.</t>
         </is>
       </c>
-      <c r="N549" s="293" t="n"/>
-      <c r="O549" s="293" t="n"/>
-      <c r="P549" s="293" t="n"/>
-      <c r="Q549" s="293" t="n"/>
-      <c r="R549" s="293" t="n"/>
-      <c r="S549" s="293" t="n"/>
-      <c r="T549" s="293" t="n"/>
-      <c r="U549" s="293" t="n"/>
-      <c r="V549" s="293" t="n"/>
-      <c r="W549" s="293" t="n"/>
-      <c r="X549" s="293" t="n"/>
-      <c r="Y549" s="293" t="n"/>
-      <c r="Z549" s="293" t="n"/>
-      <c r="AA549" s="294" t="n"/>
+      <c r="N549" s="291" t="n"/>
+      <c r="O549" s="291" t="n"/>
+      <c r="P549" s="291" t="n"/>
+      <c r="Q549" s="291" t="n"/>
+      <c r="R549" s="291" t="n"/>
+      <c r="S549" s="291" t="n"/>
+      <c r="T549" s="291" t="n"/>
+      <c r="U549" s="291" t="n"/>
+      <c r="V549" s="291" t="n"/>
+      <c r="W549" s="291" t="n"/>
+      <c r="X549" s="291" t="n"/>
+      <c r="Y549" s="291" t="n"/>
+      <c r="Z549" s="291" t="n"/>
+      <c r="AA549" s="292" t="n"/>
       <c r="AB549" s="16" t="n"/>
       <c r="AC549" s="16" t="n"/>
       <c r="AD549" s="16" t="n"/>
@@ -61836,34 +61426,34 @@
       <c r="E550" s="16" t="n"/>
       <c r="F550" s="16" t="n"/>
       <c r="G550" s="16" t="n"/>
-      <c r="H550" s="292" t="inlineStr">
+      <c r="H550" s="290" t="inlineStr">
         <is>
           <t>Variable Operating Expenses ($/MWh)</t>
         </is>
       </c>
-      <c r="I550" s="293" t="n"/>
-      <c r="J550" s="293" t="n"/>
-      <c r="K550" s="293" t="n"/>
-      <c r="L550" s="294" t="n"/>
-      <c r="M550" s="295" t="inlineStr">
+      <c r="I550" s="291" t="n"/>
+      <c r="J550" s="291" t="n"/>
+      <c r="K550" s="291" t="n"/>
+      <c r="L550" s="292" t="n"/>
+      <c r="M550" s="293" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="N550" s="293" t="n"/>
-      <c r="O550" s="293" t="n"/>
-      <c r="P550" s="293" t="n"/>
-      <c r="Q550" s="293" t="n"/>
-      <c r="R550" s="293" t="n"/>
-      <c r="S550" s="293" t="n"/>
-      <c r="T550" s="293" t="n"/>
-      <c r="U550" s="293" t="n"/>
-      <c r="V550" s="293" t="n"/>
-      <c r="W550" s="293" t="n"/>
-      <c r="X550" s="293" t="n"/>
-      <c r="Y550" s="293" t="n"/>
-      <c r="Z550" s="293" t="n"/>
-      <c r="AA550" s="296" t="n"/>
+      <c r="N550" s="291" t="n"/>
+      <c r="O550" s="291" t="n"/>
+      <c r="P550" s="291" t="n"/>
+      <c r="Q550" s="291" t="n"/>
+      <c r="R550" s="291" t="n"/>
+      <c r="S550" s="291" t="n"/>
+      <c r="T550" s="291" t="n"/>
+      <c r="U550" s="291" t="n"/>
+      <c r="V550" s="291" t="n"/>
+      <c r="W550" s="291" t="n"/>
+      <c r="X550" s="291" t="n"/>
+      <c r="Y550" s="291" t="n"/>
+      <c r="Z550" s="291" t="n"/>
+      <c r="AA550" s="294" t="n"/>
       <c r="AB550" s="16" t="n"/>
       <c r="AC550" s="16" t="n"/>
       <c r="AD550" s="16" t="n"/>
@@ -61911,34 +61501,34 @@
       <c r="E551" s="16" t="n"/>
       <c r="F551" s="16" t="n"/>
       <c r="G551" s="16" t="n"/>
-      <c r="H551" s="299" t="inlineStr">
+      <c r="H551" s="297" t="inlineStr">
         <is>
           <t>Grid Connection Cost ($/kW)</t>
         </is>
       </c>
-      <c r="I551" s="300" t="n"/>
-      <c r="J551" s="300" t="n"/>
-      <c r="K551" s="300" t="n"/>
-      <c r="L551" s="301" t="n"/>
-      <c r="M551" s="302" t="inlineStr">
+      <c r="I551" s="298" t="n"/>
+      <c r="J551" s="298" t="n"/>
+      <c r="K551" s="298" t="n"/>
+      <c r="L551" s="299" t="n"/>
+      <c r="M551" s="300" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="N551" s="300" t="n"/>
-      <c r="O551" s="300" t="n"/>
-      <c r="P551" s="300" t="n"/>
-      <c r="Q551" s="300" t="n"/>
-      <c r="R551" s="300" t="n"/>
-      <c r="S551" s="300" t="n"/>
-      <c r="T551" s="300" t="n"/>
-      <c r="U551" s="300" t="n"/>
-      <c r="V551" s="300" t="n"/>
-      <c r="W551" s="300" t="n"/>
-      <c r="X551" s="300" t="n"/>
-      <c r="Y551" s="300" t="n"/>
-      <c r="Z551" s="300" t="n"/>
-      <c r="AA551" s="303" t="n"/>
+      <c r="N551" s="298" t="n"/>
+      <c r="O551" s="298" t="n"/>
+      <c r="P551" s="298" t="n"/>
+      <c r="Q551" s="298" t="n"/>
+      <c r="R551" s="298" t="n"/>
+      <c r="S551" s="298" t="n"/>
+      <c r="T551" s="298" t="n"/>
+      <c r="U551" s="298" t="n"/>
+      <c r="V551" s="298" t="n"/>
+      <c r="W551" s="298" t="n"/>
+      <c r="X551" s="298" t="n"/>
+      <c r="Y551" s="298" t="n"/>
+      <c r="Z551" s="298" t="n"/>
+      <c r="AA551" s="301" t="n"/>
       <c r="AB551" s="16" t="n"/>
       <c r="AC551" s="16" t="n"/>
       <c r="AD551" s="16" t="n"/>

</xml_diff>